<commit_message>
Updated German league 2019
</commit_message>
<xml_diff>
--- a/data/2019-German-League/iaf short.xlsx
+++ b/data/2019-German-League/iaf short.xlsx
@@ -5,10 +5,10 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Program Files (x86)\cygwin64\home\s.hein\tmpvalet\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Program Files (x86)\cygwin64\home\s.hein\GitHub\Valet\data\2019-German-League\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C424459A-B13F-4152-8489-5DE6361D3717}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{47F1D241-D5F8-474F-8AFA-C20C4FBC60C8}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="1418" yWindow="-98" windowWidth="19199" windowHeight="13875" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -19,7 +19,7 @@
     <definedName name="_xlnm.Print_Area" localSheetId="0">iaf!$A$1:$J$147</definedName>
     <definedName name="_xlnm.Print_Titles" localSheetId="0">iaf!$1:$2</definedName>
   </definedNames>
-  <calcPr calcId="145621"/>
+  <calcPr calcId="181029"/>
 </workbook>
 </file>
 
@@ -188,9 +188,6 @@
     <t>Annaig Della Monta - Dr. Alfred Berthold</t>
   </si>
   <si>
-    <t>Herr Jokisch - Herr U, Kasimir</t>
-  </si>
-  <si>
     <t>Henning Bohnsack - Bernd Donner</t>
   </si>
   <si>
@@ -413,9 +410,6 @@
     <t>Ingo Lüßmann - Claudia Lüßmann</t>
   </si>
   <si>
-    <t>Avram Kreisberger - Ulrich Däullary</t>
-  </si>
-  <si>
     <t>Ludger Silva - Michael Böcker</t>
   </si>
   <si>
@@ -488,9 +482,6 @@
     <t>Michael Schröder - Stefan Vernon</t>
   </si>
   <si>
-    <t>Fred Wrobel - Stefan Häßler</t>
-  </si>
-  <si>
     <t>Ria Kürschner - Dr. Anne Gromöller</t>
   </si>
   <si>
@@ -501,6 +492,15 @@
   </si>
   <si>
     <t>3b</t>
+  </si>
+  <si>
+    <t>Avram Kreisberger - Ulrich DÃ¤ullary</t>
+  </si>
+  <si>
+    <t>Fred Wrobel - Stefan HÃ¤ÃŸler</t>
+  </si>
+  <si>
+    <t>Herr Jokisch - Herr U. Kasimir</t>
   </si>
 </sst>
 </file>
@@ -657,7 +657,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="37">
+  <fills count="34">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -841,24 +841,6 @@
       <patternFill patternType="solid">
         <fgColor theme="1"/>
         <bgColor theme="1"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FF00B0F0"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FF92D050"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFC000"/>
-        <bgColor indexed="64"/>
       </patternFill>
     </fill>
   </fills>
@@ -1075,7 +1057,7 @@
     <xf numFmtId="0" fontId="1" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="17" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="19">
+  <cellXfs count="20">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -1093,19 +1075,26 @@
     <xf numFmtId="0" fontId="13" fillId="33" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="19" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="19" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="13" fillId="33" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="13" fillId="33" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="13" fillId="33" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="13" fillId="33" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="13" fillId="33" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="18" fillId="35" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="18" fillId="36" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="18" fillId="34" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="right"/>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="42">
@@ -1152,7 +1141,7 @@
     <cellStyle name="Warnender Text" xfId="14" builtinId="11" customBuiltin="1"/>
     <cellStyle name="Zelle überprüfen" xfId="13" builtinId="23" customBuiltin="1"/>
   </cellStyles>
-  <dxfs count="12">
+  <dxfs count="32">
     <dxf>
       <font>
         <b val="0"/>
@@ -1169,6 +1158,147 @@
         <name val="Calibri"/>
         <scheme val="minor"/>
       </font>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF92D050"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF00B0F0"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF00B0F0"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF00B0F0"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF92D050"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF00B0F0"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF00B0F0"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF00B0F0"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF00B0F0"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF00B0F0"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF92D050"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF00B0F0"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF92D050"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF92D050"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF92D050"/>
+        </patternFill>
+      </fill>
     </dxf>
     <dxf>
       <font>
@@ -1317,21 +1447,21 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{00000000-000C-0000-FFFF-FFFF00000000}" name="Tabelle1" displayName="Tabelle1" ref="A2:J147" totalsRowShown="0" headerRowDxfId="11" dataDxfId="10" tableBorderDxfId="9">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{00000000-000C-0000-FFFF-FFFF00000000}" name="Tabelle1" displayName="Tabelle1" ref="A2:J147" totalsRowShown="0" headerRowDxfId="31" dataDxfId="30" tableBorderDxfId="29">
   <autoFilter ref="A2:J147" xr:uid="{00000000-0009-0000-0100-000001000000}"/>
   <sortState ref="A3:I35">
     <sortCondition descending="1" ref="C2:C35"/>
   </sortState>
   <tableColumns count="10">
-    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0000-000001000000}" name="Players" dataDxfId="8"/>
+    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0000-000001000000}" name="Players" dataDxfId="28"/>
     <tableColumn id="2" xr3:uid="{00000000-0010-0000-0000-000002000000}" name="Count"/>
-    <tableColumn id="3" xr3:uid="{00000000-0010-0000-0000-000003000000}" name="Butler" dataDxfId="7"/>
-    <tableColumn id="4" xr3:uid="{00000000-0010-0000-0000-000004000000}" name="Bid" dataDxfId="6"/>
-    <tableColumn id="5" xr3:uid="{00000000-0010-0000-0000-000005000000}" name="Play" dataDxfId="5"/>
-    <tableColumn id="6" xr3:uid="{00000000-0010-0000-0000-000006000000}" name="Decl" dataDxfId="4"/>
-    <tableColumn id="7" xr3:uid="{00000000-0010-0000-0000-000007000000}" name="#" dataDxfId="3"/>
-    <tableColumn id="8" xr3:uid="{00000000-0010-0000-0000-000008000000}" name="Def" dataDxfId="2"/>
-    <tableColumn id="9" xr3:uid="{00000000-0010-0000-0000-000009000000}" name=" #" dataDxfId="1"/>
+    <tableColumn id="3" xr3:uid="{00000000-0010-0000-0000-000003000000}" name="Butler" dataDxfId="27"/>
+    <tableColumn id="4" xr3:uid="{00000000-0010-0000-0000-000004000000}" name="Bid" dataDxfId="26"/>
+    <tableColumn id="5" xr3:uid="{00000000-0010-0000-0000-000005000000}" name="Play" dataDxfId="25"/>
+    <tableColumn id="6" xr3:uid="{00000000-0010-0000-0000-000006000000}" name="Decl" dataDxfId="24"/>
+    <tableColumn id="7" xr3:uid="{00000000-0010-0000-0000-000007000000}" name="#" dataDxfId="23"/>
+    <tableColumn id="8" xr3:uid="{00000000-0010-0000-0000-000008000000}" name="Def" dataDxfId="22"/>
+    <tableColumn id="9" xr3:uid="{00000000-0010-0000-0000-000009000000}" name=" #" dataDxfId="21"/>
     <tableColumn id="14" xr3:uid="{3C881E77-4381-4276-A7A4-393F008BDACD}" name="BL" dataDxfId="0"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight8" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
@@ -1604,15 +1734,15 @@
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A1:K147"/>
+  <dimension ref="A1:J147"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="B26" sqref="B26:B147"/>
+      <selection activeCell="E10" sqref="E10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
   <cols>
-    <col min="1" max="1" width="52.46484375" style="5" customWidth="1"/>
+    <col min="1" max="1" width="45.265625" style="5" customWidth="1"/>
     <col min="2" max="2" width="8" customWidth="1"/>
     <col min="3" max="3" width="7.86328125" style="7" customWidth="1"/>
     <col min="4" max="4" width="6.33203125" style="3" customWidth="1"/>
@@ -1621,24 +1751,24 @@
     <col min="7" max="7" width="5" style="8" customWidth="1"/>
     <col min="8" max="8" width="6.33203125" style="3" customWidth="1"/>
     <col min="9" max="9" width="5" style="9" customWidth="1"/>
-    <col min="10" max="10" width="5.86328125" customWidth="1"/>
+    <col min="10" max="10" width="5.86328125" style="19" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" x14ac:dyDescent="0.45">
+    <row r="1" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A1" s="10"/>
       <c r="B1" s="10"/>
       <c r="C1" s="10"/>
       <c r="D1" s="10"/>
       <c r="E1" s="10"/>
-      <c r="F1" s="15" t="s">
+      <c r="F1" s="13" t="s">
         <v>8</v>
       </c>
-      <c r="G1" s="13"/>
-      <c r="H1" s="13"/>
-      <c r="I1" s="14"/>
-      <c r="J1" s="10"/>
-    </row>
-    <row r="2" spans="1:11" s="1" customFormat="1" x14ac:dyDescent="0.45">
+      <c r="G1" s="14"/>
+      <c r="H1" s="14"/>
+      <c r="I1" s="15"/>
+      <c r="J1" s="16"/>
+    </row>
+    <row r="2" spans="1:10" s="1" customFormat="1" x14ac:dyDescent="0.45">
       <c r="A2" s="4" t="s">
         <v>0</v>
       </c>
@@ -1666,14 +1796,13 @@
       <c r="I2" s="6" t="s">
         <v>9</v>
       </c>
-      <c r="J2" s="2" t="s">
+      <c r="J2" s="17" t="s">
         <v>10</v>
       </c>
-      <c r="K2" s="2"/>
-    </row>
-    <row r="3" spans="1:11" x14ac:dyDescent="0.45">
+    </row>
+    <row r="3" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A3" s="5" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="B3">
         <v>96</v>
@@ -1699,23 +1828,22 @@
       <c r="I3" s="9">
         <v>48</v>
       </c>
-      <c r="J3" s="16">
+      <c r="J3" s="18">
         <v>1</v>
       </c>
-      <c r="K3" s="3"/>
-    </row>
-    <row r="4" spans="1:11" x14ac:dyDescent="0.45">
+    </row>
+    <row r="4" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A4" s="5" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="B4">
         <v>208</v>
       </c>
       <c r="C4" s="7">
-        <v>0.95</v>
+        <v>0.93</v>
       </c>
       <c r="D4" s="3">
-        <v>0.57999999999999996</v>
+        <v>0.56999999999999995</v>
       </c>
       <c r="E4" s="7">
         <v>0.36</v>
@@ -1732,14 +1860,13 @@
       <c r="I4" s="9">
         <v>96</v>
       </c>
-      <c r="J4" s="16">
+      <c r="J4" s="18">
         <v>1</v>
       </c>
-      <c r="K4" s="3"/>
-    </row>
-    <row r="5" spans="1:11" x14ac:dyDescent="0.45">
+    </row>
+    <row r="5" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A5" s="5" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="B5">
         <v>112</v>
@@ -1765,14 +1892,13 @@
       <c r="I5" s="9">
         <v>61</v>
       </c>
-      <c r="J5" s="16">
+      <c r="J5" s="18">
         <v>1</v>
       </c>
-      <c r="K5" s="3"/>
-    </row>
-    <row r="6" spans="1:11" x14ac:dyDescent="0.45">
+    </row>
+    <row r="6" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A6" s="5" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="B6">
         <v>192</v>
@@ -1787,7 +1913,7 @@
         <v>0.13</v>
       </c>
       <c r="F6" s="3">
-        <v>0.11</v>
+        <v>0.12</v>
       </c>
       <c r="G6" s="11">
         <v>104</v>
@@ -1798,142 +1924,139 @@
       <c r="I6" s="12">
         <v>88</v>
       </c>
-      <c r="J6" s="17">
+      <c r="J6" s="18">
         <v>2</v>
       </c>
-      <c r="K6" s="3"/>
-    </row>
-    <row r="7" spans="1:11" x14ac:dyDescent="0.45">
+    </row>
+    <row r="7" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A7" s="5" t="s">
+        <v>37</v>
+      </c>
+      <c r="B7">
+        <v>96</v>
+      </c>
+      <c r="C7" s="7">
+        <v>0.64</v>
+      </c>
+      <c r="D7" s="3">
+        <v>0.33</v>
+      </c>
+      <c r="E7" s="7">
+        <v>0.3</v>
+      </c>
+      <c r="F7" s="3">
+        <v>0.67</v>
+      </c>
+      <c r="G7" s="8">
+        <v>43</v>
+      </c>
+      <c r="H7" s="3">
+        <v>0</v>
+      </c>
+      <c r="I7" s="9">
+        <v>53</v>
+      </c>
+      <c r="J7" s="18" t="s">
+        <v>155</v>
+      </c>
+    </row>
+    <row r="8" spans="1:10" x14ac:dyDescent="0.45">
+      <c r="A8" s="5" t="s">
         <v>25</v>
       </c>
-      <c r="B7">
+      <c r="B8">
         <v>288</v>
       </c>
-      <c r="C7" s="7">
+      <c r="C8" s="7">
         <v>0.63</v>
       </c>
-      <c r="D7" s="3">
+      <c r="D8" s="3">
         <v>0.18</v>
       </c>
-      <c r="E7" s="7">
+      <c r="E8" s="7">
         <v>0.46</v>
       </c>
-      <c r="F7" s="3">
+      <c r="F8" s="3">
         <v>0.64</v>
       </c>
-      <c r="G7" s="8">
+      <c r="G8" s="11">
         <v>147</v>
       </c>
-      <c r="H7" s="3">
-        <v>0.27</v>
-      </c>
-      <c r="I7" s="9">
+      <c r="H8" s="3">
+        <v>0.28000000000000003</v>
+      </c>
+      <c r="I8" s="12">
         <v>139</v>
       </c>
-      <c r="J7" s="18" t="s">
+      <c r="J8" s="18" t="s">
         <v>23</v>
       </c>
     </row>
-    <row r="8" spans="1:11" x14ac:dyDescent="0.45">
-      <c r="A8" s="5" t="s">
+    <row r="9" spans="1:10" x14ac:dyDescent="0.45">
+      <c r="A9" s="5" t="s">
         <v>36</v>
-      </c>
-      <c r="B8">
-        <v>96</v>
-      </c>
-      <c r="C8" s="7">
-        <v>0.62</v>
-      </c>
-      <c r="D8" s="3">
-        <v>0.43</v>
-      </c>
-      <c r="E8" s="7">
-        <v>0.2</v>
-      </c>
-      <c r="F8" s="3">
-        <v>0.01</v>
-      </c>
-      <c r="G8" s="11">
-        <v>41</v>
-      </c>
-      <c r="H8" s="3">
-        <v>0.34</v>
-      </c>
-      <c r="I8" s="12">
-        <v>54</v>
-      </c>
-      <c r="J8" s="18" t="s">
-        <v>157</v>
-      </c>
-      <c r="K8" s="3"/>
-    </row>
-    <row r="9" spans="1:11" x14ac:dyDescent="0.45">
-      <c r="A9" s="5" t="s">
-        <v>37</v>
       </c>
       <c r="B9">
         <v>96</v>
       </c>
       <c r="C9" s="7">
-        <v>0.61</v>
+        <v>0.62</v>
       </c>
       <c r="D9" s="3">
-        <v>0.31</v>
+        <v>0.43</v>
       </c>
       <c r="E9" s="7">
-        <v>0.3</v>
+        <v>0.19</v>
       </c>
       <c r="F9" s="3">
-        <v>0.68</v>
+        <v>0.01</v>
       </c>
       <c r="G9" s="11">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="H9" s="3">
-        <v>0</v>
+        <v>0.33</v>
       </c>
       <c r="I9" s="12">
-        <v>53</v>
+        <v>54</v>
       </c>
       <c r="J9" s="18" t="s">
-        <v>158</v>
-      </c>
-      <c r="K9" s="3"/>
-    </row>
-    <row r="10" spans="1:11" x14ac:dyDescent="0.45">
+        <v>154</v>
+      </c>
+    </row>
+    <row r="10" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A10" s="5" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="B10">
-        <v>160</v>
+        <v>208</v>
       </c>
       <c r="C10" s="7">
-        <v>0.6</v>
+        <v>0.59</v>
       </c>
       <c r="D10" s="3">
-        <v>0.56999999999999995</v>
+        <v>0.27</v>
       </c>
       <c r="E10" s="7">
-        <v>0.03</v>
+        <v>0.32</v>
       </c>
       <c r="F10" s="3">
-        <v>-0.12</v>
+        <v>0.23</v>
       </c>
       <c r="G10" s="11">
-        <v>82</v>
+        <v>99</v>
       </c>
       <c r="H10" s="3">
-        <v>0.19</v>
+        <v>0.4</v>
       </c>
       <c r="I10" s="12">
-        <v>78</v>
+        <v>108</v>
       </c>
       <c r="J10" s="18" t="s">
-        <v>158</v>
-      </c>
-    </row>
-    <row r="11" spans="1:11" x14ac:dyDescent="0.45">
+        <v>155</v>
+      </c>
+    </row>
+    <row r="11" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A11" s="5" t="s">
         <v>12</v>
       </c>
@@ -1941,22 +2064,22 @@
         <v>287</v>
       </c>
       <c r="C11" s="7">
-        <v>0.6</v>
+        <v>0.57999999999999996</v>
       </c>
       <c r="D11" s="3">
-        <v>0.35</v>
+        <v>0.34</v>
       </c>
       <c r="E11" s="7">
         <v>0.24</v>
       </c>
       <c r="F11" s="3">
-        <v>0.51</v>
+        <v>0.5</v>
       </c>
       <c r="G11" s="8">
         <v>154</v>
       </c>
       <c r="H11" s="3">
-        <v>-0.06</v>
+        <v>-7.0000000000000007E-2</v>
       </c>
       <c r="I11" s="9">
         <v>132</v>
@@ -1965,39 +2088,39 @@
         <v>23</v>
       </c>
     </row>
-    <row r="12" spans="1:11" x14ac:dyDescent="0.45">
+    <row r="12" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A12" s="5" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="B12">
-        <v>208</v>
+        <v>160</v>
       </c>
       <c r="C12" s="7">
         <v>0.57999999999999996</v>
       </c>
       <c r="D12" s="3">
-        <v>0.26</v>
+        <v>0.55000000000000004</v>
       </c>
       <c r="E12" s="7">
-        <v>0.32</v>
+        <v>0.03</v>
       </c>
       <c r="F12" s="3">
-        <v>0.23</v>
+        <v>-0.12</v>
       </c>
       <c r="G12" s="8">
-        <v>99</v>
+        <v>82</v>
       </c>
       <c r="H12" s="3">
-        <v>0.4</v>
+        <v>0.19</v>
       </c>
       <c r="I12" s="9">
-        <v>108</v>
+        <v>78</v>
       </c>
       <c r="J12" s="18" t="s">
-        <v>158</v>
-      </c>
-    </row>
-    <row r="13" spans="1:11" x14ac:dyDescent="0.45">
+        <v>155</v>
+      </c>
+    </row>
+    <row r="13" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A13" s="5" t="s">
         <v>40</v>
       </c>
@@ -2005,16 +2128,16 @@
         <v>192</v>
       </c>
       <c r="C13" s="7">
-        <v>0.56999999999999995</v>
+        <v>0.56000000000000005</v>
       </c>
       <c r="D13" s="3">
-        <v>-0.05</v>
+        <v>-0.04</v>
       </c>
       <c r="E13" s="7">
-        <v>0.62</v>
+        <v>0.59</v>
       </c>
       <c r="F13" s="3">
-        <v>0.91</v>
+        <v>0.87</v>
       </c>
       <c r="G13" s="8">
         <v>97</v>
@@ -2026,10 +2149,10 @@
         <v>95</v>
       </c>
       <c r="J13" s="18" t="s">
-        <v>157</v>
-      </c>
-    </row>
-    <row r="14" spans="1:11" x14ac:dyDescent="0.45">
+        <v>154</v>
+      </c>
+    </row>
+    <row r="14" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A14" s="5" t="s">
         <v>24</v>
       </c>
@@ -2043,7 +2166,7 @@
         <v>0.28000000000000003</v>
       </c>
       <c r="E14" s="7">
-        <v>0.27</v>
+        <v>0.28000000000000003</v>
       </c>
       <c r="F14" s="3">
         <v>0.4</v>
@@ -2061,7 +2184,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="15" spans="1:11" x14ac:dyDescent="0.45">
+    <row r="15" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A15" s="5" t="s">
         <v>41</v>
       </c>
@@ -2069,10 +2192,10 @@
         <v>272</v>
       </c>
       <c r="C15" s="7">
-        <v>0.53</v>
+        <v>0.54</v>
       </c>
       <c r="D15" s="3">
-        <v>0.17</v>
+        <v>0.18</v>
       </c>
       <c r="E15" s="7">
         <v>0.36</v>
@@ -2089,11 +2212,11 @@
       <c r="I15" s="9">
         <v>130</v>
       </c>
-      <c r="J15" s="16">
+      <c r="J15" s="18">
         <v>1</v>
       </c>
     </row>
-    <row r="16" spans="1:11" x14ac:dyDescent="0.45">
+    <row r="16" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A16" s="5" t="s">
         <v>42</v>
       </c>
@@ -2110,7 +2233,7 @@
         <v>0.66</v>
       </c>
       <c r="F16" s="3">
-        <v>0.94</v>
+        <v>0.95</v>
       </c>
       <c r="G16" s="11">
         <v>53</v>
@@ -2121,7 +2244,7 @@
       <c r="I16" s="12">
         <v>40</v>
       </c>
-      <c r="J16" s="17">
+      <c r="J16" s="18">
         <v>2</v>
       </c>
     </row>
@@ -2154,7 +2277,7 @@
         <v>78</v>
       </c>
       <c r="J17" s="18" t="s">
-        <v>158</v>
+        <v>155</v>
       </c>
     </row>
     <row r="18" spans="1:10" x14ac:dyDescent="0.45">
@@ -2165,7 +2288,7 @@
         <v>128</v>
       </c>
       <c r="C18" s="7">
-        <v>0.51</v>
+        <v>0.5</v>
       </c>
       <c r="D18" s="3">
         <v>0.16</v>
@@ -2185,7 +2308,7 @@
       <c r="I18" s="9">
         <v>63</v>
       </c>
-      <c r="J18" s="17">
+      <c r="J18" s="18">
         <v>2</v>
       </c>
     </row>
@@ -2217,40 +2340,40 @@
       <c r="I19" s="9">
         <v>98</v>
       </c>
-      <c r="J19" s="17">
+      <c r="J19" s="18">
         <v>2</v>
       </c>
     </row>
     <row r="20" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A20" s="5" t="s">
-        <v>129</v>
+        <v>47</v>
       </c>
       <c r="B20">
-        <v>112</v>
+        <v>192</v>
       </c>
       <c r="C20" s="7">
-        <v>0.48</v>
+        <v>0.49</v>
       </c>
       <c r="D20" s="3">
-        <v>0.28000000000000003</v>
+        <v>0.26</v>
       </c>
       <c r="E20" s="7">
-        <v>0.2</v>
+        <v>0.23</v>
       </c>
       <c r="F20" s="3">
-        <v>-0.03</v>
+        <v>0.1</v>
       </c>
       <c r="G20" s="11">
-        <v>53</v>
+        <v>95</v>
       </c>
       <c r="H20" s="3">
-        <v>0.41</v>
+        <v>0.36</v>
       </c>
       <c r="I20" s="12">
-        <v>58</v>
+        <v>96</v>
       </c>
       <c r="J20" s="18" t="s">
-        <v>157</v>
+        <v>154</v>
       </c>
     </row>
     <row r="21" spans="1:10" x14ac:dyDescent="0.45">
@@ -2264,13 +2387,13 @@
         <v>0.48</v>
       </c>
       <c r="D21" s="3">
-        <v>0.43</v>
+        <v>0.44</v>
       </c>
       <c r="E21" s="7">
         <v>0.05</v>
       </c>
       <c r="F21" s="3">
-        <v>-0.17</v>
+        <v>-0.18</v>
       </c>
       <c r="G21" s="8">
         <v>116</v>
@@ -2282,15 +2405,15 @@
         <v>107</v>
       </c>
       <c r="J21" s="18" t="s">
-        <v>157</v>
+        <v>154</v>
       </c>
     </row>
     <row r="22" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A22" s="5" t="s">
-        <v>47</v>
+        <v>11</v>
       </c>
       <c r="B22">
-        <v>192</v>
+        <v>288</v>
       </c>
       <c r="C22" s="7">
         <v>0.47</v>
@@ -2302,51 +2425,51 @@
         <v>0.22</v>
       </c>
       <c r="F22" s="3">
-        <v>0.09</v>
+        <v>0.21</v>
       </c>
       <c r="G22" s="8">
-        <v>95</v>
+        <v>119</v>
       </c>
       <c r="H22" s="3">
-        <v>0.36</v>
+        <v>0.24</v>
       </c>
       <c r="I22" s="9">
-        <v>96</v>
+        <v>167</v>
       </c>
       <c r="J22" s="18" t="s">
-        <v>157</v>
+        <v>23</v>
       </c>
     </row>
     <row r="23" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A23" s="5" t="s">
-        <v>11</v>
+        <v>156</v>
       </c>
       <c r="B23">
-        <v>288</v>
+        <v>112</v>
       </c>
       <c r="C23" s="7">
         <v>0.47</v>
       </c>
       <c r="D23" s="3">
-        <v>0.24</v>
+        <v>0.27</v>
       </c>
       <c r="E23" s="7">
-        <v>0.22</v>
+        <v>0.2</v>
       </c>
       <c r="F23" s="3">
-        <v>0.21</v>
+        <v>-0.03</v>
       </c>
       <c r="G23" s="11">
-        <v>119</v>
+        <v>53</v>
       </c>
       <c r="H23" s="3">
-        <v>0.24</v>
+        <v>0.41</v>
       </c>
       <c r="I23" s="12">
-        <v>167</v>
+        <v>58</v>
       </c>
       <c r="J23" s="18" t="s">
-        <v>23</v>
+        <v>154</v>
       </c>
     </row>
     <row r="24" spans="1:10" x14ac:dyDescent="0.45">
@@ -2377,13 +2500,13 @@
       <c r="I24" s="9">
         <v>125</v>
       </c>
-      <c r="J24" s="17">
+      <c r="J24" s="18">
         <v>2</v>
       </c>
     </row>
     <row r="25" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A25" s="5" t="s">
-        <v>130</v>
+        <v>128</v>
       </c>
       <c r="B25">
         <v>192</v>
@@ -2410,7 +2533,7 @@
         <v>93</v>
       </c>
       <c r="J25" s="18" t="s">
-        <v>157</v>
+        <v>154</v>
       </c>
     </row>
     <row r="26" spans="1:10" x14ac:dyDescent="0.45">
@@ -2450,7 +2573,7 @@
         <v>49</v>
       </c>
       <c r="B27">
-        <v>174</v>
+        <v>127</v>
       </c>
       <c r="C27" s="7">
         <v>0.43</v>
@@ -2468,13 +2591,13 @@
         <v>62</v>
       </c>
       <c r="H27" s="3">
-        <v>0.7</v>
+        <v>0.69</v>
       </c>
       <c r="I27" s="12">
         <v>63</v>
       </c>
       <c r="J27" s="18" t="s">
-        <v>157</v>
+        <v>154</v>
       </c>
     </row>
     <row r="28" spans="1:10" x14ac:dyDescent="0.45">
@@ -2482,7 +2605,7 @@
         <v>50</v>
       </c>
       <c r="B28">
-        <v>174</v>
+        <v>96</v>
       </c>
       <c r="C28" s="7">
         <v>0.4</v>
@@ -2491,7 +2614,7 @@
         <v>-0.01</v>
       </c>
       <c r="E28" s="7">
-        <v>0.41</v>
+        <v>0.4</v>
       </c>
       <c r="F28" s="3">
         <v>0.22</v>
@@ -2505,176 +2628,176 @@
       <c r="I28" s="12">
         <v>46</v>
       </c>
-      <c r="J28" s="17">
+      <c r="J28" s="18">
         <v>2</v>
       </c>
     </row>
     <row r="29" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A29" s="5" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="B29">
-        <v>174</v>
+        <v>192</v>
       </c>
       <c r="C29" s="7">
-        <v>0.4</v>
+        <v>0.39</v>
       </c>
       <c r="D29" s="3">
-        <v>0.36</v>
+        <v>-0.06</v>
       </c>
       <c r="E29" s="7">
-        <v>0.04</v>
+        <v>0.45</v>
       </c>
       <c r="F29" s="3">
-        <v>0.14000000000000001</v>
+        <v>0.28000000000000003</v>
       </c>
       <c r="G29" s="11">
-        <v>59</v>
+        <v>101</v>
       </c>
       <c r="H29" s="3">
-        <v>-0.08</v>
+        <v>0.65</v>
       </c>
       <c r="I29" s="12">
-        <v>52</v>
-      </c>
-      <c r="J29" s="16">
-        <v>1</v>
+        <v>90</v>
+      </c>
+      <c r="J29" s="18" t="s">
+        <v>154</v>
       </c>
     </row>
     <row r="30" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A30" s="5" t="s">
-        <v>132</v>
+        <v>51</v>
       </c>
       <c r="B30">
-        <v>174</v>
+        <v>144</v>
       </c>
       <c r="C30" s="7">
-        <v>0.38</v>
+        <v>0.39</v>
       </c>
       <c r="D30" s="3">
-        <v>-0.04</v>
+        <v>-0.15</v>
       </c>
       <c r="E30" s="7">
-        <v>0.43</v>
+        <v>0.54</v>
       </c>
       <c r="F30" s="3">
-        <v>0.28000000000000003</v>
+        <v>0.53</v>
       </c>
       <c r="G30" s="8">
-        <v>101</v>
+        <v>61</v>
       </c>
       <c r="H30" s="3">
-        <v>0.6</v>
+        <v>0.54</v>
       </c>
       <c r="I30" s="9">
-        <v>90</v>
+        <v>83</v>
       </c>
       <c r="J30" s="18" t="s">
-        <v>157</v>
+        <v>155</v>
       </c>
     </row>
     <row r="31" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A31" s="5" t="s">
-        <v>51</v>
+        <v>129</v>
       </c>
       <c r="B31">
-        <v>174</v>
+        <v>111</v>
       </c>
       <c r="C31" s="7">
-        <v>0.38</v>
+        <v>0.39</v>
       </c>
       <c r="D31" s="3">
-        <v>-0.16</v>
+        <v>0.36</v>
       </c>
       <c r="E31" s="7">
-        <v>0.54</v>
+        <v>0.04</v>
       </c>
       <c r="F31" s="3">
-        <v>0.53</v>
+        <v>0.14000000000000001</v>
       </c>
       <c r="G31" s="8">
-        <v>61</v>
+        <v>59</v>
       </c>
       <c r="H31" s="3">
-        <v>0.55000000000000004</v>
+        <v>-0.08</v>
       </c>
       <c r="I31" s="9">
-        <v>83</v>
-      </c>
-      <c r="J31" s="18" t="s">
-        <v>158</v>
+        <v>52</v>
+      </c>
+      <c r="J31" s="18">
+        <v>1</v>
       </c>
     </row>
     <row r="32" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A32" s="5" t="s">
-        <v>52</v>
+        <v>53</v>
       </c>
       <c r="B32">
-        <v>174</v>
+        <v>192</v>
       </c>
       <c r="C32" s="7">
         <v>0.38</v>
       </c>
       <c r="D32" s="3">
-        <v>0.11</v>
+        <v>0.03</v>
       </c>
       <c r="E32" s="7">
-        <v>0.26</v>
+        <v>0.36</v>
       </c>
       <c r="F32" s="3">
-        <v>0.27</v>
+        <v>0.05</v>
       </c>
       <c r="G32" s="11">
-        <v>44</v>
+        <v>87</v>
       </c>
       <c r="H32" s="3">
-        <v>0.27</v>
+        <v>0.62</v>
       </c>
       <c r="I32" s="12">
-        <v>51</v>
+        <v>104</v>
       </c>
       <c r="J32" s="18" t="s">
-        <v>158</v>
+        <v>154</v>
       </c>
     </row>
     <row r="33" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A33" s="5" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="B33">
-        <v>174</v>
+        <v>96</v>
       </c>
       <c r="C33" s="7">
-        <v>0.37</v>
+        <v>0.38</v>
       </c>
       <c r="D33" s="3">
-        <v>0.01</v>
+        <v>0.12</v>
       </c>
       <c r="E33" s="7">
-        <v>0.36</v>
+        <v>0.26</v>
       </c>
       <c r="F33" s="3">
-        <v>0.05</v>
+        <v>0.27</v>
       </c>
       <c r="G33" s="11">
-        <v>87</v>
+        <v>44</v>
       </c>
       <c r="H33" s="3">
-        <v>0.62</v>
+        <v>0.27</v>
       </c>
       <c r="I33" s="12">
-        <v>104</v>
+        <v>51</v>
       </c>
       <c r="J33" s="18" t="s">
-        <v>157</v>
+        <v>155</v>
       </c>
     </row>
     <row r="34" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A34" s="5" t="s">
-        <v>133</v>
+        <v>131</v>
       </c>
       <c r="B34">
-        <v>174</v>
+        <v>128</v>
       </c>
       <c r="C34" s="7">
         <v>0.37</v>
@@ -2683,7 +2806,7 @@
         <v>0.46</v>
       </c>
       <c r="E34" s="7">
-        <v>-0.1</v>
+        <v>-0.09</v>
       </c>
       <c r="F34" s="3">
         <v>0.17</v>
@@ -2697,25 +2820,25 @@
       <c r="I34" s="9">
         <v>71</v>
       </c>
-      <c r="J34" s="17">
+      <c r="J34" s="18">
         <v>2</v>
       </c>
     </row>
     <row r="35" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A35" s="5" t="s">
-        <v>54</v>
+        <v>158</v>
       </c>
       <c r="B35">
-        <v>174</v>
+        <v>208</v>
       </c>
       <c r="C35" s="7">
-        <v>0.35</v>
+        <v>0.34</v>
       </c>
       <c r="D35" s="3">
         <v>0.5</v>
       </c>
       <c r="E35" s="7">
-        <v>-0.15</v>
+        <v>-0.16</v>
       </c>
       <c r="F35" s="3">
         <v>-0.26</v>
@@ -2724,30 +2847,30 @@
         <v>105</v>
       </c>
       <c r="H35" s="3">
-        <v>-0.04</v>
+        <v>-0.05</v>
       </c>
       <c r="I35" s="12">
         <v>103</v>
       </c>
-      <c r="J35" s="16">
+      <c r="J35" s="18">
         <v>1</v>
       </c>
     </row>
     <row r="36" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A36" s="5" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="B36">
-        <v>174</v>
+        <v>176</v>
       </c>
       <c r="C36" s="7">
-        <v>0.32</v>
+        <v>0.33</v>
       </c>
       <c r="D36" s="3">
         <v>0.26</v>
       </c>
       <c r="E36" s="7">
-        <v>0.06</v>
+        <v>7.0000000000000007E-2</v>
       </c>
       <c r="F36" s="3">
         <v>0.06</v>
@@ -2756,13 +2879,13 @@
         <v>99</v>
       </c>
       <c r="H36" s="3">
-        <v>7.0000000000000007E-2</v>
+        <v>0.08</v>
       </c>
       <c r="I36" s="9">
         <v>77</v>
       </c>
       <c r="J36" s="18" t="s">
-        <v>158</v>
+        <v>155</v>
       </c>
     </row>
     <row r="37" spans="1:10" x14ac:dyDescent="0.45">
@@ -2770,159 +2893,159 @@
         <v>56</v>
       </c>
       <c r="B37">
-        <v>174</v>
+        <v>128</v>
       </c>
       <c r="C37" s="7">
-        <v>0.31</v>
+        <v>0.32</v>
       </c>
       <c r="D37" s="3">
-        <v>0.23</v>
+        <v>0.33</v>
       </c>
       <c r="E37" s="7">
-        <v>0.08</v>
+        <v>0</v>
       </c>
       <c r="F37" s="3">
-        <v>0.25</v>
+        <v>-0.23</v>
       </c>
       <c r="G37" s="8">
-        <v>130</v>
+        <v>66</v>
       </c>
       <c r="H37" s="3">
-        <v>-0.09</v>
+        <v>0.24</v>
       </c>
       <c r="I37" s="9">
-        <v>121</v>
-      </c>
-      <c r="J37" s="17">
-        <v>2</v>
+        <v>62</v>
+      </c>
+      <c r="J37" s="18">
+        <v>1</v>
       </c>
     </row>
     <row r="38" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A38" s="5" t="s">
-        <v>134</v>
+        <v>58</v>
       </c>
       <c r="B38">
-        <v>174</v>
+        <v>140</v>
       </c>
       <c r="C38" s="7">
-        <v>0.31</v>
+        <v>0.32</v>
       </c>
       <c r="D38" s="3">
-        <v>0.15</v>
+        <v>0.41</v>
       </c>
       <c r="E38" s="7">
-        <v>0.16</v>
+        <v>-0.09</v>
       </c>
       <c r="F38" s="3">
-        <v>0.54</v>
+        <v>-0.15</v>
       </c>
       <c r="G38" s="8">
-        <v>118</v>
+        <v>74</v>
       </c>
       <c r="H38" s="3">
-        <v>-0.27</v>
+        <v>-0.03</v>
       </c>
       <c r="I38" s="9">
-        <v>103</v>
-      </c>
-      <c r="J38" s="16">
+        <v>65</v>
+      </c>
+      <c r="J38" s="18">
         <v>1</v>
       </c>
     </row>
     <row r="39" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A39" s="5" t="s">
-        <v>57</v>
+        <v>132</v>
       </c>
       <c r="B39">
-        <v>174</v>
+        <v>222</v>
       </c>
       <c r="C39" s="7">
-        <v>0.3</v>
+        <v>0.32</v>
       </c>
       <c r="D39" s="3">
-        <v>0.31</v>
+        <v>0.15</v>
       </c>
       <c r="E39" s="7">
-        <v>-0.01</v>
+        <v>0.16</v>
       </c>
       <c r="F39" s="3">
-        <v>-0.23</v>
+        <v>0.54</v>
       </c>
       <c r="G39" s="8">
-        <v>66</v>
+        <v>118</v>
       </c>
       <c r="H39" s="3">
-        <v>0.24</v>
+        <v>-0.27</v>
       </c>
       <c r="I39" s="9">
-        <v>62</v>
-      </c>
-      <c r="J39" s="16">
+        <v>103</v>
+      </c>
+      <c r="J39" s="18">
         <v>1</v>
       </c>
     </row>
     <row r="40" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A40" s="5" t="s">
-        <v>58</v>
+        <v>55</v>
       </c>
       <c r="B40">
-        <v>174</v>
+        <v>254</v>
       </c>
       <c r="C40" s="7">
-        <v>0.3</v>
+        <v>0.32</v>
       </c>
       <c r="D40" s="3">
-        <v>0.31</v>
+        <v>0.23</v>
       </c>
       <c r="E40" s="7">
-        <v>-0.01</v>
+        <v>0.08</v>
       </c>
       <c r="F40" s="3">
-        <v>0.17</v>
+        <v>0.25</v>
       </c>
       <c r="G40" s="8">
-        <v>126</v>
+        <v>130</v>
       </c>
       <c r="H40" s="3">
-        <v>-0.21</v>
+        <v>-0.1</v>
       </c>
       <c r="I40" s="9">
-        <v>112</v>
-      </c>
-      <c r="J40" s="18" t="s">
-        <v>158</v>
+        <v>121</v>
+      </c>
+      <c r="J40" s="18">
+        <v>2</v>
       </c>
     </row>
     <row r="41" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A41" s="5" t="s">
-        <v>135</v>
+        <v>57</v>
       </c>
       <c r="B41">
-        <v>174</v>
+        <v>240</v>
       </c>
       <c r="C41" s="7">
         <v>0.3</v>
       </c>
       <c r="D41" s="3">
-        <v>0.3</v>
+        <v>0.31</v>
       </c>
       <c r="E41" s="7">
-        <v>0</v>
+        <v>-0.01</v>
       </c>
       <c r="F41" s="3">
-        <v>-0.12</v>
+        <v>0.17</v>
       </c>
       <c r="G41" s="8">
-        <v>137</v>
+        <v>126</v>
       </c>
       <c r="H41" s="3">
-        <v>0.16</v>
+        <v>-0.21</v>
       </c>
       <c r="I41" s="9">
-        <v>103</v>
+        <v>112</v>
       </c>
       <c r="J41" s="18" t="s">
-        <v>157</v>
+        <v>155</v>
       </c>
     </row>
     <row r="42" spans="1:10" x14ac:dyDescent="0.45">
@@ -2930,159 +3053,159 @@
         <v>59</v>
       </c>
       <c r="B42">
-        <v>174</v>
+        <v>176</v>
       </c>
       <c r="C42" s="7">
         <v>0.3</v>
       </c>
       <c r="D42" s="3">
-        <v>0.4</v>
+        <v>0.56999999999999995</v>
       </c>
       <c r="E42" s="7">
-        <v>-0.1</v>
+        <v>-0.27</v>
       </c>
       <c r="F42" s="3">
-        <v>-0.16</v>
+        <v>-0.34</v>
       </c>
       <c r="G42" s="8">
-        <v>74</v>
+        <v>81</v>
       </c>
       <c r="H42" s="3">
-        <v>-0.03</v>
+        <v>-0.22</v>
       </c>
       <c r="I42" s="9">
-        <v>65</v>
-      </c>
-      <c r="J42" s="16">
-        <v>1</v>
+        <v>94</v>
+      </c>
+      <c r="J42" s="18" t="s">
+        <v>155</v>
       </c>
     </row>
     <row r="43" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A43" s="5" t="s">
-        <v>60</v>
+        <v>133</v>
       </c>
       <c r="B43">
-        <v>174</v>
+        <v>240</v>
       </c>
       <c r="C43" s="7">
-        <v>0.3</v>
+        <v>0.28999999999999998</v>
       </c>
       <c r="D43" s="3">
-        <v>0.56999999999999995</v>
+        <v>0.31</v>
       </c>
       <c r="E43" s="7">
-        <v>-0.28000000000000003</v>
+        <v>-0.02</v>
       </c>
       <c r="F43" s="3">
-        <v>-0.35</v>
+        <v>-0.15</v>
       </c>
       <c r="G43" s="8">
-        <v>81</v>
+        <v>137</v>
       </c>
       <c r="H43" s="3">
-        <v>-0.22</v>
+        <v>0.16</v>
       </c>
       <c r="I43" s="9">
-        <v>94</v>
+        <v>103</v>
       </c>
       <c r="J43" s="18" t="s">
-        <v>158</v>
+        <v>154</v>
       </c>
     </row>
     <row r="44" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A44" s="5" t="s">
-        <v>28</v>
+        <v>60</v>
       </c>
       <c r="B44">
-        <v>174</v>
+        <v>144</v>
       </c>
       <c r="C44" s="7">
+        <v>0.28999999999999998</v>
+      </c>
+      <c r="D44" s="3">
         <v>0.28000000000000003</v>
       </c>
-      <c r="D44" s="3">
-        <v>0.32</v>
-      </c>
       <c r="E44" s="7">
-        <v>-0.03</v>
+        <v>0.01</v>
       </c>
       <c r="F44" s="3">
-        <v>-0.32</v>
+        <v>-0.1</v>
       </c>
       <c r="G44" s="8">
-        <v>96</v>
+        <v>76</v>
       </c>
       <c r="H44" s="3">
-        <v>0.25</v>
+        <v>0.13</v>
       </c>
       <c r="I44" s="9">
-        <v>96</v>
+        <v>68</v>
       </c>
       <c r="J44" s="18" t="s">
-        <v>23</v>
+        <v>155</v>
       </c>
     </row>
     <row r="45" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A45" s="5" t="s">
-        <v>61</v>
+        <v>134</v>
       </c>
       <c r="B45">
-        <v>174</v>
+        <v>192</v>
       </c>
       <c r="C45" s="7">
         <v>0.28000000000000003</v>
       </c>
       <c r="D45" s="3">
-        <v>0.27</v>
+        <v>0.25</v>
       </c>
       <c r="E45" s="7">
-        <v>0.01</v>
+        <v>0.03</v>
       </c>
       <c r="F45" s="3">
-        <v>-0.1</v>
+        <v>0.34</v>
       </c>
       <c r="G45" s="8">
-        <v>76</v>
+        <v>91</v>
       </c>
       <c r="H45" s="3">
-        <v>0.13</v>
+        <v>-0.26</v>
       </c>
       <c r="I45" s="9">
-        <v>68</v>
+        <v>99</v>
       </c>
       <c r="J45" s="18" t="s">
-        <v>158</v>
+        <v>155</v>
       </c>
     </row>
     <row r="46" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A46" s="5" t="s">
-        <v>136</v>
+        <v>28</v>
       </c>
       <c r="B46">
-        <v>174</v>
+        <v>192</v>
       </c>
       <c r="C46" s="7">
-        <v>0.28000000000000003</v>
+        <v>0.27</v>
       </c>
       <c r="D46" s="3">
+        <v>0.3</v>
+      </c>
+      <c r="E46" s="7">
+        <v>-0.03</v>
+      </c>
+      <c r="F46" s="3">
+        <v>-0.31</v>
+      </c>
+      <c r="G46" s="8">
+        <v>96</v>
+      </c>
+      <c r="H46" s="3">
         <v>0.25</v>
       </c>
-      <c r="E46" s="7">
-        <v>0.03</v>
-      </c>
-      <c r="F46" s="3">
-        <v>0.34</v>
-      </c>
-      <c r="G46" s="8">
-        <v>91</v>
-      </c>
-      <c r="H46" s="3">
-        <v>-0.25</v>
-      </c>
       <c r="I46" s="9">
-        <v>99</v>
+        <v>96</v>
       </c>
       <c r="J46" s="18" t="s">
-        <v>158</v>
+        <v>23</v>
       </c>
     </row>
     <row r="47" spans="1:10" x14ac:dyDescent="0.45">
@@ -3090,7 +3213,7 @@
         <v>27</v>
       </c>
       <c r="B47">
-        <v>174</v>
+        <v>176</v>
       </c>
       <c r="C47" s="7">
         <v>0.27</v>
@@ -3119,10 +3242,10 @@
     </row>
     <row r="48" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A48" s="5" t="s">
-        <v>153</v>
+        <v>151</v>
       </c>
       <c r="B48">
-        <v>174</v>
+        <v>192</v>
       </c>
       <c r="C48" s="7">
         <v>0.27</v>
@@ -3146,15 +3269,15 @@
         <v>88</v>
       </c>
       <c r="J48" s="18" t="s">
-        <v>157</v>
+        <v>154</v>
       </c>
     </row>
     <row r="49" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A49" s="5" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="B49">
-        <v>174</v>
+        <v>128</v>
       </c>
       <c r="C49" s="7">
         <v>0.24</v>
@@ -3178,21 +3301,21 @@
         <v>71</v>
       </c>
       <c r="J49" s="18" t="s">
-        <v>157</v>
+        <v>154</v>
       </c>
     </row>
     <row r="50" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A50" s="5" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="B50">
-        <v>174</v>
+        <v>192</v>
       </c>
       <c r="C50" s="7">
-        <v>0.24</v>
+        <v>0.23</v>
       </c>
       <c r="D50" s="3">
-        <v>0.03</v>
+        <v>0.02</v>
       </c>
       <c r="E50" s="7">
         <v>0.21</v>
@@ -3209,72 +3332,72 @@
       <c r="I50" s="9">
         <v>87</v>
       </c>
-      <c r="J50" s="16">
+      <c r="J50" s="18">
         <v>1</v>
       </c>
     </row>
     <row r="51" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A51" s="5" t="s">
-        <v>64</v>
+        <v>30</v>
       </c>
       <c r="B51">
-        <v>174</v>
+        <v>287</v>
       </c>
       <c r="C51" s="7">
         <v>0.22</v>
       </c>
       <c r="D51" s="3">
-        <v>0.06</v>
+        <v>-0.09</v>
       </c>
       <c r="E51" s="7">
-        <v>0.17</v>
+        <v>0.32</v>
       </c>
       <c r="F51" s="3">
-        <v>0.34</v>
+        <v>0.36</v>
       </c>
       <c r="G51" s="8">
-        <v>135</v>
+        <v>148</v>
       </c>
       <c r="H51" s="3">
-        <v>0.02</v>
+        <v>0.28000000000000003</v>
       </c>
       <c r="I51" s="9">
-        <v>152</v>
+        <v>137</v>
       </c>
       <c r="J51" s="18" t="s">
-        <v>158</v>
+        <v>23</v>
       </c>
     </row>
     <row r="52" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A52" s="5" t="s">
-        <v>30</v>
+        <v>64</v>
       </c>
       <c r="B52">
-        <v>174</v>
+        <v>192</v>
       </c>
       <c r="C52" s="7">
         <v>0.22</v>
       </c>
       <c r="D52" s="3">
-        <v>-0.09</v>
+        <v>0.09</v>
       </c>
       <c r="E52" s="7">
-        <v>0.32</v>
+        <v>0.13</v>
       </c>
       <c r="F52" s="3">
-        <v>0.36</v>
+        <v>0.18</v>
       </c>
       <c r="G52" s="8">
-        <v>148</v>
+        <v>92</v>
       </c>
       <c r="H52" s="3">
-        <v>0.28000000000000003</v>
+        <v>0.09</v>
       </c>
       <c r="I52" s="9">
-        <v>137</v>
+        <v>100</v>
       </c>
       <c r="J52" s="18" t="s">
-        <v>23</v>
+        <v>154</v>
       </c>
     </row>
     <row r="53" spans="1:10" x14ac:dyDescent="0.45">
@@ -3282,71 +3405,71 @@
         <v>65</v>
       </c>
       <c r="B53">
-        <v>174</v>
+        <v>192</v>
       </c>
       <c r="C53" s="7">
         <v>0.22</v>
       </c>
       <c r="D53" s="3">
-        <v>0.09</v>
+        <v>0.35</v>
       </c>
       <c r="E53" s="7">
-        <v>0.14000000000000001</v>
+        <v>-0.13</v>
       </c>
       <c r="F53" s="3">
-        <v>0.19</v>
+        <v>7.0000000000000007E-2</v>
       </c>
       <c r="G53" s="8">
-        <v>92</v>
+        <v>86</v>
       </c>
       <c r="H53" s="3">
-        <v>0.09</v>
+        <v>-0.3</v>
       </c>
       <c r="I53" s="9">
-        <v>100</v>
-      </c>
-      <c r="J53" s="18" t="s">
-        <v>157</v>
+        <v>104</v>
+      </c>
+      <c r="J53" s="18">
+        <v>1</v>
       </c>
     </row>
     <row r="54" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A54" s="5" t="s">
-        <v>66</v>
+        <v>63</v>
       </c>
       <c r="B54">
-        <v>174</v>
+        <v>288</v>
       </c>
       <c r="C54" s="7">
         <v>0.22</v>
       </c>
       <c r="D54" s="3">
-        <v>0.35</v>
+        <v>0.05</v>
       </c>
       <c r="E54" s="7">
-        <v>-0.13</v>
+        <v>0.17</v>
       </c>
       <c r="F54" s="3">
-        <v>7.0000000000000007E-2</v>
+        <v>0.34</v>
       </c>
       <c r="G54" s="8">
-        <v>86</v>
+        <v>135</v>
       </c>
       <c r="H54" s="3">
-        <v>-0.3</v>
+        <v>0.02</v>
       </c>
       <c r="I54" s="9">
-        <v>104</v>
-      </c>
-      <c r="J54" s="16">
-        <v>1</v>
+        <v>152</v>
+      </c>
+      <c r="J54" s="18" t="s">
+        <v>155</v>
       </c>
     </row>
     <row r="55" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A55" s="5" t="s">
-        <v>154</v>
+        <v>157</v>
       </c>
       <c r="B55">
-        <v>174</v>
+        <v>176</v>
       </c>
       <c r="C55" s="7">
         <v>0.21</v>
@@ -3358,7 +3481,7 @@
         <v>0.47</v>
       </c>
       <c r="F55" s="3">
-        <v>0.5</v>
+        <v>0.51</v>
       </c>
       <c r="G55" s="8">
         <v>88</v>
@@ -3369,16 +3492,16 @@
       <c r="I55" s="9">
         <v>88</v>
       </c>
-      <c r="J55" s="17">
+      <c r="J55" s="18">
         <v>2</v>
       </c>
     </row>
     <row r="56" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A56" s="5" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="B56">
-        <v>174</v>
+        <v>208</v>
       </c>
       <c r="C56" s="7">
         <v>0.21</v>
@@ -3396,13 +3519,13 @@
         <v>112</v>
       </c>
       <c r="H56" s="3">
-        <v>0.03</v>
+        <v>0.02</v>
       </c>
       <c r="I56" s="9">
         <v>95</v>
       </c>
       <c r="J56" s="18" t="s">
-        <v>158</v>
+        <v>155</v>
       </c>
     </row>
     <row r="57" spans="1:10" x14ac:dyDescent="0.45">
@@ -3410,7 +3533,7 @@
         <v>13</v>
       </c>
       <c r="B57">
-        <v>174</v>
+        <v>192</v>
       </c>
       <c r="C57" s="7">
         <v>0.2</v>
@@ -3439,10 +3562,10 @@
     </row>
     <row r="58" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A58" s="5" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="B58">
-        <v>174</v>
+        <v>144</v>
       </c>
       <c r="C58" s="7">
         <v>0.18</v>
@@ -3466,18 +3589,18 @@
         <v>76</v>
       </c>
       <c r="J58" s="18" t="s">
-        <v>158</v>
+        <v>155</v>
       </c>
     </row>
     <row r="59" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A59" s="5" t="s">
-        <v>137</v>
+        <v>135</v>
       </c>
       <c r="B59">
-        <v>174</v>
+        <v>272</v>
       </c>
       <c r="C59" s="7">
-        <v>0.16</v>
+        <v>0.17</v>
       </c>
       <c r="D59" s="3">
         <v>0.04</v>
@@ -3498,15 +3621,15 @@
         <v>121</v>
       </c>
       <c r="J59" s="18" t="s">
-        <v>158</v>
+        <v>155</v>
       </c>
     </row>
     <row r="60" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A60" s="5" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="B60">
-        <v>174</v>
+        <v>256</v>
       </c>
       <c r="C60" s="7">
         <v>0.16</v>
@@ -3524,27 +3647,27 @@
         <v>133</v>
       </c>
       <c r="H60" s="3">
-        <v>0</v>
+        <v>0.01</v>
       </c>
       <c r="I60" s="9">
         <v>121</v>
       </c>
-      <c r="J60" s="16">
+      <c r="J60" s="18">
         <v>1</v>
       </c>
     </row>
     <row r="61" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A61" s="5" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="B61">
-        <v>174</v>
+        <v>192</v>
       </c>
       <c r="C61" s="7">
-        <v>0.15</v>
+        <v>0.16</v>
       </c>
       <c r="D61" s="3">
-        <v>0.22</v>
+        <v>0.24</v>
       </c>
       <c r="E61" s="7">
         <v>-0.08</v>
@@ -3556,30 +3679,30 @@
         <v>106</v>
       </c>
       <c r="H61" s="3">
-        <v>-0.25</v>
+        <v>-0.26</v>
       </c>
       <c r="I61" s="9">
         <v>85</v>
       </c>
-      <c r="J61" s="17">
+      <c r="J61" s="18">
         <v>2</v>
       </c>
     </row>
     <row r="62" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A62" s="5" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="B62">
-        <v>174</v>
+        <v>192</v>
       </c>
       <c r="C62" s="7">
-        <v>0.14000000000000001</v>
+        <v>0.15</v>
       </c>
       <c r="D62" s="3">
-        <v>0.05</v>
+        <v>0.04</v>
       </c>
       <c r="E62" s="7">
-        <v>0.09</v>
+        <v>0.11</v>
       </c>
       <c r="F62" s="3">
         <v>-0.23</v>
@@ -3588,21 +3711,21 @@
         <v>89</v>
       </c>
       <c r="H62" s="3">
-        <v>0.36</v>
+        <v>0.41</v>
       </c>
       <c r="I62" s="9">
         <v>102</v>
       </c>
       <c r="J62" s="18" t="s">
-        <v>157</v>
+        <v>154</v>
       </c>
     </row>
     <row r="63" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A63" s="5" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="B63">
-        <v>174</v>
+        <v>192</v>
       </c>
       <c r="C63" s="7">
         <v>0.13</v>
@@ -3626,85 +3749,85 @@
         <v>98</v>
       </c>
       <c r="J63" s="18" t="s">
-        <v>158</v>
+        <v>155</v>
       </c>
     </row>
     <row r="64" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A64" s="5" t="s">
-        <v>73</v>
+        <v>136</v>
       </c>
       <c r="B64">
-        <v>174</v>
+        <v>128</v>
       </c>
       <c r="C64" s="7">
-        <v>0.11</v>
+        <v>0.13</v>
       </c>
       <c r="D64" s="3">
-        <v>-0.14000000000000001</v>
+        <v>0.19</v>
       </c>
       <c r="E64" s="7">
-        <v>0.26</v>
+        <v>-0.06</v>
       </c>
       <c r="F64" s="3">
-        <v>0.01</v>
+        <v>0.15</v>
       </c>
       <c r="G64" s="8">
-        <v>89</v>
+        <v>66</v>
       </c>
       <c r="H64" s="3">
-        <v>0.52</v>
+        <v>-0.28999999999999998</v>
       </c>
       <c r="I64" s="9">
-        <v>86</v>
-      </c>
-      <c r="J64" s="16">
-        <v>1</v>
+        <v>61</v>
+      </c>
+      <c r="J64" s="18" t="s">
+        <v>154</v>
       </c>
     </row>
     <row r="65" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A65" s="5" t="s">
-        <v>138</v>
+        <v>72</v>
       </c>
       <c r="B65">
-        <v>174</v>
+        <v>176</v>
       </c>
       <c r="C65" s="7">
         <v>0.11</v>
       </c>
       <c r="D65" s="3">
-        <v>0.18</v>
+        <v>-0.14000000000000001</v>
       </c>
       <c r="E65" s="7">
-        <v>-7.0000000000000007E-2</v>
+        <v>0.26</v>
       </c>
       <c r="F65" s="3">
-        <v>0.15</v>
+        <v>0.01</v>
       </c>
       <c r="G65" s="8">
-        <v>66</v>
+        <v>89</v>
       </c>
       <c r="H65" s="3">
-        <v>-0.31</v>
+        <v>0.52</v>
       </c>
       <c r="I65" s="9">
-        <v>61</v>
-      </c>
-      <c r="J65" s="18" t="s">
-        <v>157</v>
+        <v>86</v>
+      </c>
+      <c r="J65" s="18">
+        <v>1</v>
       </c>
     </row>
     <row r="66" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A66" s="5" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="B66">
-        <v>174</v>
+        <v>256</v>
       </c>
       <c r="C66" s="7">
         <v>0.11</v>
       </c>
       <c r="D66" s="3">
-        <v>-0.1</v>
+        <v>-0.11</v>
       </c>
       <c r="E66" s="7">
         <v>0.21</v>
@@ -3721,40 +3844,40 @@
       <c r="I66" s="9">
         <v>129</v>
       </c>
-      <c r="J66" s="16">
+      <c r="J66" s="18">
         <v>1</v>
       </c>
     </row>
     <row r="67" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A67" s="5" t="s">
-        <v>75</v>
+        <v>31</v>
       </c>
       <c r="B67">
-        <v>174</v>
+        <v>176</v>
       </c>
       <c r="C67" s="7">
         <v>0.1</v>
       </c>
       <c r="D67" s="3">
-        <v>7.0000000000000007E-2</v>
+        <v>0.17</v>
       </c>
       <c r="E67" s="7">
-        <v>0.03</v>
+        <v>-7.0000000000000007E-2</v>
       </c>
       <c r="F67" s="3">
-        <v>0.27</v>
+        <v>0.13</v>
       </c>
       <c r="G67" s="8">
-        <v>99</v>
+        <v>79</v>
       </c>
       <c r="H67" s="3">
-        <v>-0.22</v>
+        <v>-0.23</v>
       </c>
       <c r="I67" s="9">
-        <v>92</v>
-      </c>
-      <c r="J67" s="17">
-        <v>2</v>
+        <v>96</v>
+      </c>
+      <c r="J67" s="18" t="s">
+        <v>23</v>
       </c>
     </row>
     <row r="68" spans="1:10" x14ac:dyDescent="0.45">
@@ -3762,7 +3885,7 @@
         <v>14</v>
       </c>
       <c r="B68">
-        <v>174</v>
+        <v>206</v>
       </c>
       <c r="C68" s="7">
         <v>0.1</v>
@@ -3774,7 +3897,7 @@
         <v>-7.0000000000000007E-2</v>
       </c>
       <c r="F68" s="3">
-        <v>-0.22</v>
+        <v>-0.21</v>
       </c>
       <c r="G68" s="8">
         <v>100</v>
@@ -3791,19 +3914,19 @@
     </row>
     <row r="69" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A69" s="5" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="B69">
-        <v>174</v>
+        <v>223</v>
       </c>
       <c r="C69" s="7">
-        <v>0.1</v>
+        <v>0.09</v>
       </c>
       <c r="D69" s="3">
         <v>0.18</v>
       </c>
       <c r="E69" s="7">
-        <v>-0.08</v>
+        <v>-0.09</v>
       </c>
       <c r="F69" s="3">
         <v>0.03</v>
@@ -3812,13 +3935,13 @@
         <v>115</v>
       </c>
       <c r="H69" s="3">
-        <v>-0.19</v>
+        <v>-0.2</v>
       </c>
       <c r="I69" s="9">
         <v>108</v>
       </c>
       <c r="J69" s="18" t="s">
-        <v>158</v>
+        <v>155</v>
       </c>
     </row>
     <row r="70" spans="1:10" x14ac:dyDescent="0.45">
@@ -3826,7 +3949,7 @@
         <v>16</v>
       </c>
       <c r="B70">
-        <v>174</v>
+        <v>288</v>
       </c>
       <c r="C70" s="7">
         <v>0.09</v>
@@ -3855,48 +3978,48 @@
     </row>
     <row r="71" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A71" s="5" t="s">
-        <v>31</v>
+        <v>74</v>
       </c>
       <c r="B71">
-        <v>174</v>
+        <v>192</v>
       </c>
       <c r="C71" s="7">
-        <v>0.08</v>
+        <v>0.09</v>
       </c>
       <c r="D71" s="3">
-        <v>0.15</v>
+        <v>0.06</v>
       </c>
       <c r="E71" s="7">
-        <v>-7.0000000000000007E-2</v>
+        <v>0.03</v>
       </c>
       <c r="F71" s="3">
-        <v>0.13</v>
+        <v>0.27</v>
       </c>
       <c r="G71" s="8">
-        <v>79</v>
+        <v>99</v>
       </c>
       <c r="H71" s="3">
         <v>-0.23</v>
       </c>
       <c r="I71" s="9">
-        <v>96</v>
-      </c>
-      <c r="J71" s="18" t="s">
-        <v>23</v>
+        <v>92</v>
+      </c>
+      <c r="J71" s="18">
+        <v>2</v>
       </c>
     </row>
     <row r="72" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A72" s="5" t="s">
-        <v>156</v>
+        <v>153</v>
       </c>
       <c r="B72">
-        <v>174</v>
+        <v>191</v>
       </c>
       <c r="C72" s="7">
-        <v>0.08</v>
+        <v>7.0000000000000007E-2</v>
       </c>
       <c r="D72" s="3">
-        <v>0.22</v>
+        <v>0.2</v>
       </c>
       <c r="E72" s="7">
         <v>-0.13</v>
@@ -3914,71 +4037,71 @@
         <v>89</v>
       </c>
       <c r="J72" s="18" t="s">
-        <v>157</v>
+        <v>154</v>
       </c>
     </row>
     <row r="73" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A73" s="5" t="s">
-        <v>77</v>
+        <v>78</v>
       </c>
       <c r="B73">
-        <v>174</v>
+        <v>112</v>
       </c>
       <c r="C73" s="7">
         <v>0.06</v>
       </c>
       <c r="D73" s="3">
-        <v>-0.3</v>
+        <v>0.17</v>
       </c>
       <c r="E73" s="7">
-        <v>0.36</v>
+        <v>-0.11</v>
       </c>
       <c r="F73" s="3">
-        <v>0.65</v>
+        <v>0.19</v>
       </c>
       <c r="G73" s="8">
-        <v>72</v>
+        <v>60</v>
       </c>
       <c r="H73" s="3">
-        <v>-0.02</v>
+        <v>-0.48</v>
       </c>
       <c r="I73" s="9">
-        <v>56</v>
-      </c>
-      <c r="J73" s="16">
-        <v>1</v>
+        <v>50</v>
+      </c>
+      <c r="J73" s="18" t="s">
+        <v>154</v>
       </c>
     </row>
     <row r="74" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A74" s="5" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
       <c r="B74">
-        <v>174</v>
+        <v>128</v>
       </c>
       <c r="C74" s="7">
-        <v>0.05</v>
+        <v>0.06</v>
       </c>
       <c r="D74" s="3">
-        <v>-0.01</v>
+        <v>-0.3</v>
       </c>
       <c r="E74" s="7">
-        <v>0.06</v>
+        <v>0.36</v>
       </c>
       <c r="F74" s="3">
-        <v>0.03</v>
+        <v>0.65</v>
       </c>
       <c r="G74" s="8">
-        <v>96</v>
+        <v>72</v>
       </c>
       <c r="H74" s="3">
-        <v>0.09</v>
+        <v>-0.02</v>
       </c>
       <c r="I74" s="9">
-        <v>95</v>
-      </c>
-      <c r="J74" s="17">
-        <v>2</v>
+        <v>56</v>
+      </c>
+      <c r="J74" s="18">
+        <v>1</v>
       </c>
     </row>
     <row r="75" spans="1:10" x14ac:dyDescent="0.45">
@@ -3986,95 +4109,95 @@
         <v>79</v>
       </c>
       <c r="B75">
-        <v>174</v>
+        <v>191</v>
       </c>
       <c r="C75" s="7">
-        <v>0.04</v>
+        <v>0.05</v>
       </c>
       <c r="D75" s="3">
-        <v>0.15</v>
+        <v>0</v>
       </c>
       <c r="E75" s="7">
-        <v>-0.11</v>
+        <v>0.05</v>
       </c>
       <c r="F75" s="3">
-        <v>0.19</v>
+        <v>-0.1</v>
       </c>
       <c r="G75" s="8">
-        <v>60</v>
+        <v>88</v>
       </c>
       <c r="H75" s="3">
-        <v>-0.48</v>
+        <v>0.18</v>
       </c>
       <c r="I75" s="9">
-        <v>50</v>
-      </c>
-      <c r="J75" s="18" t="s">
-        <v>157</v>
+        <v>102</v>
+      </c>
+      <c r="J75" s="18">
+        <v>2</v>
       </c>
     </row>
     <row r="76" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A76" s="5" t="s">
-        <v>17</v>
+        <v>77</v>
       </c>
       <c r="B76">
-        <v>174</v>
+        <v>192</v>
       </c>
       <c r="C76" s="7">
+        <v>0.04</v>
+      </c>
+      <c r="D76" s="3">
+        <v>-0.02</v>
+      </c>
+      <c r="E76" s="7">
+        <v>0.06</v>
+      </c>
+      <c r="F76" s="3">
         <v>0.03</v>
       </c>
-      <c r="D76" s="3">
-        <v>-0.2</v>
-      </c>
-      <c r="E76" s="7">
-        <v>0.24</v>
-      </c>
-      <c r="F76" s="3">
-        <v>0.16</v>
-      </c>
       <c r="G76" s="8">
-        <v>87</v>
+        <v>96</v>
       </c>
       <c r="H76" s="3">
-        <v>0.3</v>
+        <v>0.09</v>
       </c>
       <c r="I76" s="9">
-        <v>103</v>
-      </c>
-      <c r="J76" s="18" t="s">
-        <v>23</v>
+        <v>95</v>
+      </c>
+      <c r="J76" s="18">
+        <v>2</v>
       </c>
     </row>
     <row r="77" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A77" s="5" t="s">
-        <v>80</v>
+        <v>17</v>
       </c>
       <c r="B77">
-        <v>174</v>
+        <v>191</v>
       </c>
       <c r="C77" s="7">
         <v>0.03</v>
       </c>
       <c r="D77" s="3">
-        <v>-0.01</v>
+        <v>-0.2</v>
       </c>
       <c r="E77" s="7">
-        <v>0.05</v>
+        <v>0.23</v>
       </c>
       <c r="F77" s="3">
-        <v>-0.1</v>
+        <v>0.16</v>
       </c>
       <c r="G77" s="8">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="H77" s="3">
-        <v>0.18</v>
+        <v>0.3</v>
       </c>
       <c r="I77" s="9">
-        <v>102</v>
-      </c>
-      <c r="J77" s="17">
-        <v>2</v>
+        <v>103</v>
+      </c>
+      <c r="J77" s="18" t="s">
+        <v>23</v>
       </c>
     </row>
     <row r="78" spans="1:10" x14ac:dyDescent="0.45">
@@ -4082,7 +4205,7 @@
         <v>29</v>
       </c>
       <c r="B78">
-        <v>174</v>
+        <v>288</v>
       </c>
       <c r="C78" s="7">
         <v>0.03</v>
@@ -4094,7 +4217,7 @@
         <v>0.06</v>
       </c>
       <c r="F78" s="3">
-        <v>0.13</v>
+        <v>0.12</v>
       </c>
       <c r="G78" s="8">
         <v>144</v>
@@ -4111,16 +4234,16 @@
     </row>
     <row r="79" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A79" s="5" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="B79">
-        <v>174</v>
+        <v>223</v>
       </c>
       <c r="C79" s="7">
+        <v>0.02</v>
+      </c>
+      <c r="D79" s="3">
         <v>0.03</v>
-      </c>
-      <c r="D79" s="3">
-        <v>0.04</v>
       </c>
       <c r="E79" s="7">
         <v>-0.01</v>
@@ -4138,27 +4261,27 @@
         <v>122</v>
       </c>
       <c r="J79" s="18" t="s">
-        <v>158</v>
+        <v>155</v>
       </c>
     </row>
     <row r="80" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A80" s="5" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="B80">
-        <v>174</v>
+        <v>208</v>
       </c>
       <c r="C80" s="7">
-        <v>0.02</v>
+        <v>0.01</v>
       </c>
       <c r="D80" s="3">
-        <v>-0.09</v>
+        <v>-0.1</v>
       </c>
       <c r="E80" s="7">
-        <v>0.12</v>
+        <v>0.11</v>
       </c>
       <c r="F80" s="3">
-        <v>0.11</v>
+        <v>0.1</v>
       </c>
       <c r="G80" s="8">
         <v>102</v>
@@ -4170,15 +4293,15 @@
         <v>105</v>
       </c>
       <c r="J80" s="18" t="s">
-        <v>157</v>
+        <v>154</v>
       </c>
     </row>
     <row r="81" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A81" s="5" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="B81">
-        <v>174</v>
+        <v>192</v>
       </c>
       <c r="C81" s="7">
         <v>0</v>
@@ -4201,54 +4324,54 @@
       <c r="I81" s="9">
         <v>96</v>
       </c>
-      <c r="J81" s="17">
+      <c r="J81" s="18">
         <v>2</v>
       </c>
     </row>
     <row r="82" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A82" s="5" t="s">
-        <v>84</v>
+        <v>85</v>
       </c>
       <c r="B82">
         <v>174</v>
       </c>
       <c r="C82" s="7">
-        <v>0</v>
+        <v>-0.01</v>
       </c>
       <c r="D82" s="3">
-        <v>0.25</v>
+        <v>7.0000000000000007E-2</v>
       </c>
       <c r="E82" s="7">
-        <v>-0.25</v>
+        <v>-0.08</v>
       </c>
       <c r="F82" s="3">
-        <v>-0.33</v>
+        <v>0.34</v>
       </c>
       <c r="G82" s="8">
-        <v>129</v>
+        <v>86</v>
       </c>
       <c r="H82" s="3">
-        <v>-0.17</v>
+        <v>-0.5</v>
       </c>
       <c r="I82" s="9">
-        <v>111</v>
-      </c>
-      <c r="J82" s="18" t="s">
-        <v>157</v>
+        <v>88</v>
+      </c>
+      <c r="J82" s="18">
+        <v>2</v>
       </c>
     </row>
     <row r="83" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A83" s="5" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="B83">
-        <v>174</v>
+        <v>112</v>
       </c>
       <c r="C83" s="7">
-        <v>0</v>
+        <v>-0.01</v>
       </c>
       <c r="D83" s="3">
-        <v>-0.3</v>
+        <v>-0.31</v>
       </c>
       <c r="E83" s="7">
         <v>0.3</v>
@@ -4265,48 +4388,48 @@
       <c r="I83" s="9">
         <v>50</v>
       </c>
-      <c r="J83" s="17">
+      <c r="J83" s="18">
         <v>2</v>
       </c>
     </row>
     <row r="84" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A84" s="5" t="s">
-        <v>86</v>
+        <v>83</v>
       </c>
       <c r="B84">
-        <v>174</v>
+        <v>240</v>
       </c>
       <c r="C84" s="7">
-        <v>-0.01</v>
+        <v>-0.02</v>
       </c>
       <c r="D84" s="3">
-        <v>0.08</v>
+        <v>0.23</v>
       </c>
       <c r="E84" s="7">
-        <v>-0.09</v>
+        <v>-0.25</v>
       </c>
       <c r="F84" s="3">
-        <v>0.33</v>
+        <v>-0.33</v>
       </c>
       <c r="G84" s="8">
-        <v>86</v>
+        <v>129</v>
       </c>
       <c r="H84" s="3">
-        <v>-0.5</v>
+        <v>-0.17</v>
       </c>
       <c r="I84" s="9">
-        <v>88</v>
-      </c>
-      <c r="J84" s="17">
-        <v>2</v>
+        <v>111</v>
+      </c>
+      <c r="J84" s="18" t="s">
+        <v>154</v>
       </c>
     </row>
     <row r="85" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A85" s="5" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="B85">
-        <v>174</v>
+        <v>240</v>
       </c>
       <c r="C85" s="7">
         <v>-0.03</v>
@@ -4330,21 +4453,21 @@
         <v>121</v>
       </c>
       <c r="J85" s="18" t="s">
-        <v>157</v>
+        <v>154</v>
       </c>
     </row>
     <row r="86" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A86" s="5" t="s">
-        <v>151</v>
+        <v>149</v>
       </c>
       <c r="B86">
-        <v>174</v>
+        <v>176</v>
       </c>
       <c r="C86" s="7">
         <v>-0.04</v>
       </c>
       <c r="D86" s="3">
-        <v>-0.22</v>
+        <v>-0.23</v>
       </c>
       <c r="E86" s="7">
         <v>0.19</v>
@@ -4362,15 +4485,15 @@
         <v>100</v>
       </c>
       <c r="J86" s="18" t="s">
-        <v>158</v>
+        <v>155</v>
       </c>
     </row>
     <row r="87" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A87" s="5" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="B87">
-        <v>174</v>
+        <v>208</v>
       </c>
       <c r="C87" s="7">
         <v>-0.05</v>
@@ -4393,22 +4516,22 @@
       <c r="I87" s="9">
         <v>107</v>
       </c>
-      <c r="J87" s="16">
+      <c r="J87" s="18">
         <v>1</v>
       </c>
     </row>
     <row r="88" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A88" s="5" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="B88">
-        <v>174</v>
+        <v>172</v>
       </c>
       <c r="C88" s="7">
         <v>-0.05</v>
       </c>
       <c r="D88" s="3">
-        <v>0.02</v>
+        <v>0.01</v>
       </c>
       <c r="E88" s="7">
         <v>-0.06</v>
@@ -4425,156 +4548,156 @@
       <c r="I88" s="9">
         <v>79</v>
       </c>
-      <c r="J88" s="16">
+      <c r="J88" s="18">
         <v>1</v>
       </c>
     </row>
     <row r="89" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A89" s="5" t="s">
-        <v>18</v>
+        <v>89</v>
       </c>
       <c r="B89">
-        <v>174</v>
+        <v>286</v>
       </c>
       <c r="C89" s="7">
-        <v>-0.08</v>
+        <v>-7.0000000000000007E-2</v>
       </c>
       <c r="D89" s="3">
-        <v>-0.14000000000000001</v>
+        <v>-0.11</v>
       </c>
       <c r="E89" s="7">
-        <v>7.0000000000000007E-2</v>
+        <v>0.04</v>
       </c>
       <c r="F89" s="3">
-        <v>0.34</v>
+        <v>0.12</v>
       </c>
       <c r="G89" s="8">
-        <v>101</v>
+        <v>148</v>
       </c>
       <c r="H89" s="3">
-        <v>-0.25</v>
+        <v>-0.06</v>
       </c>
       <c r="I89" s="9">
-        <v>87</v>
-      </c>
-      <c r="J89" s="18" t="s">
-        <v>158</v>
+        <v>137</v>
+      </c>
+      <c r="J89" s="18">
+        <v>2</v>
       </c>
     </row>
     <row r="90" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A90" s="5" t="s">
-        <v>90</v>
+        <v>18</v>
       </c>
       <c r="B90">
-        <v>174</v>
+        <v>189</v>
       </c>
       <c r="C90" s="7">
         <v>-0.08</v>
       </c>
       <c r="D90" s="3">
-        <v>-0.12</v>
+        <v>-0.15</v>
       </c>
       <c r="E90" s="7">
-        <v>0.04</v>
+        <v>7.0000000000000007E-2</v>
       </c>
       <c r="F90" s="3">
-        <v>0.12</v>
+        <v>0.34</v>
       </c>
       <c r="G90" s="8">
-        <v>148</v>
+        <v>101</v>
       </c>
       <c r="H90" s="3">
-        <v>-0.06</v>
+        <v>-0.25</v>
       </c>
       <c r="I90" s="9">
-        <v>137</v>
-      </c>
-      <c r="J90" s="17">
-        <v>2</v>
+        <v>87</v>
+      </c>
+      <c r="J90" s="18" t="s">
+        <v>23</v>
       </c>
     </row>
     <row r="91" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A91" s="5" t="s">
-        <v>91</v>
+        <v>148</v>
       </c>
       <c r="B91">
-        <v>174</v>
+        <v>208</v>
       </c>
       <c r="C91" s="7">
+        <v>-0.08</v>
+      </c>
+      <c r="D91" s="3">
+        <v>0.01</v>
+      </c>
+      <c r="E91" s="7">
         <v>-0.09</v>
       </c>
-      <c r="D91" s="3">
-        <v>-0.23</v>
-      </c>
-      <c r="E91" s="7">
-        <v>0.14000000000000001</v>
-      </c>
       <c r="F91" s="3">
-        <v>0.15</v>
+        <v>0.01</v>
       </c>
       <c r="G91" s="8">
         <v>91</v>
       </c>
       <c r="H91" s="3">
-        <v>0.14000000000000001</v>
+        <v>-0.17</v>
       </c>
       <c r="I91" s="9">
-        <v>99</v>
+        <v>116</v>
       </c>
       <c r="J91" s="18" t="s">
-        <v>158</v>
+        <v>154</v>
       </c>
     </row>
     <row r="92" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A92" s="5" t="s">
-        <v>150</v>
+        <v>90</v>
       </c>
       <c r="B92">
-        <v>174</v>
+        <v>191</v>
       </c>
       <c r="C92" s="7">
-        <v>-0.09</v>
+        <v>-0.08</v>
       </c>
       <c r="D92" s="3">
-        <v>0.01</v>
+        <v>-0.23</v>
       </c>
       <c r="E92" s="7">
-        <v>-0.09</v>
+        <v>0.14000000000000001</v>
       </c>
       <c r="F92" s="3">
-        <v>0.01</v>
+        <v>0.15</v>
       </c>
       <c r="G92" s="8">
         <v>91</v>
       </c>
       <c r="H92" s="3">
-        <v>-0.17</v>
+        <v>0.14000000000000001</v>
       </c>
       <c r="I92" s="9">
-        <v>116</v>
+        <v>99</v>
       </c>
       <c r="J92" s="18" t="s">
-        <v>157</v>
+        <v>155</v>
       </c>
     </row>
     <row r="93" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A93" s="5" t="s">
-        <v>152</v>
+        <v>150</v>
       </c>
       <c r="B93">
-        <v>174</v>
+        <v>176</v>
       </c>
       <c r="C93" s="7">
         <v>-0.09</v>
       </c>
       <c r="D93" s="3">
-        <v>7.0000000000000007E-2</v>
+        <v>0.06</v>
       </c>
       <c r="E93" s="7">
-        <v>-0.16</v>
+        <v>-0.15</v>
       </c>
       <c r="F93" s="3">
-        <v>0</v>
+        <v>0.01</v>
       </c>
       <c r="G93" s="8">
         <v>112</v>
@@ -4586,7 +4709,7 @@
         <v>62</v>
       </c>
       <c r="J93" s="18" t="s">
-        <v>158</v>
+        <v>155</v>
       </c>
     </row>
     <row r="94" spans="1:10" x14ac:dyDescent="0.45">
@@ -4594,7 +4717,7 @@
         <v>15</v>
       </c>
       <c r="B94">
-        <v>174</v>
+        <v>190</v>
       </c>
       <c r="C94" s="7">
         <v>-0.09</v>
@@ -4623,16 +4746,16 @@
     </row>
     <row r="95" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A95" s="5" t="s">
-        <v>148</v>
+        <v>146</v>
       </c>
       <c r="B95">
-        <v>174</v>
+        <v>160</v>
       </c>
       <c r="C95" s="7">
-        <v>-0.11</v>
+        <v>-0.12</v>
       </c>
       <c r="D95" s="3">
-        <v>-0.25</v>
+        <v>-0.26</v>
       </c>
       <c r="E95" s="7">
         <v>0.14000000000000001</v>
@@ -4649,28 +4772,28 @@
       <c r="I95" s="9">
         <v>89</v>
       </c>
-      <c r="J95" s="17">
+      <c r="J95" s="18">
         <v>2</v>
       </c>
     </row>
     <row r="96" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A96" s="5" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="B96">
-        <v>174</v>
+        <v>144</v>
       </c>
       <c r="C96" s="7">
-        <v>-0.14000000000000001</v>
+        <v>-0.13</v>
       </c>
       <c r="D96" s="3">
-        <v>-0.24</v>
+        <v>-0.23</v>
       </c>
       <c r="E96" s="7">
         <v>0.1</v>
       </c>
       <c r="F96" s="3">
-        <v>-0.01</v>
+        <v>0</v>
       </c>
       <c r="G96" s="8">
         <v>66</v>
@@ -4681,7 +4804,7 @@
       <c r="I96" s="9">
         <v>77</v>
       </c>
-      <c r="J96" s="16">
+      <c r="J96" s="18">
         <v>1</v>
       </c>
     </row>
@@ -4690,7 +4813,7 @@
         <v>33</v>
       </c>
       <c r="B97">
-        <v>174</v>
+        <v>176</v>
       </c>
       <c r="C97" s="7">
         <v>-0.14000000000000001</v>
@@ -4719,10 +4842,10 @@
     </row>
     <row r="98" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A98" s="5" t="s">
-        <v>139</v>
+        <v>137</v>
       </c>
       <c r="B98">
-        <v>174</v>
+        <v>96</v>
       </c>
       <c r="C98" s="7">
         <v>-0.15</v>
@@ -4746,21 +4869,21 @@
         <v>61</v>
       </c>
       <c r="J98" s="18" t="s">
-        <v>158</v>
+        <v>155</v>
       </c>
     </row>
     <row r="99" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A99" s="5" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="B99">
-        <v>174</v>
+        <v>95</v>
       </c>
       <c r="C99" s="7">
-        <v>-0.16</v>
+        <v>-0.17</v>
       </c>
       <c r="D99" s="3">
-        <v>0.6</v>
+        <v>0.59</v>
       </c>
       <c r="E99" s="7">
         <v>-0.76</v>
@@ -4778,18 +4901,18 @@
         <v>40</v>
       </c>
       <c r="J99" s="18" t="s">
-        <v>158</v>
+        <v>155</v>
       </c>
     </row>
     <row r="100" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A100" s="5" t="s">
-        <v>149</v>
+        <v>147</v>
       </c>
       <c r="B100">
-        <v>174</v>
+        <v>192</v>
       </c>
       <c r="C100" s="7">
-        <v>-0.21</v>
+        <v>-0.2</v>
       </c>
       <c r="D100" s="3">
         <v>0</v>
@@ -4809,16 +4932,16 @@
       <c r="I100" s="9">
         <v>105</v>
       </c>
-      <c r="J100" s="16">
+      <c r="J100" s="18">
         <v>1</v>
       </c>
     </row>
     <row r="101" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A101" s="5" t="s">
-        <v>140</v>
+        <v>138</v>
       </c>
       <c r="B101">
-        <v>174</v>
+        <v>128</v>
       </c>
       <c r="C101" s="7">
         <v>-0.21</v>
@@ -4841,19 +4964,19 @@
       <c r="I101" s="9">
         <v>69</v>
       </c>
-      <c r="J101" s="16">
+      <c r="J101" s="18">
         <v>1</v>
       </c>
     </row>
     <row r="102" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A102" s="5" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="B102">
-        <v>174</v>
+        <v>223</v>
       </c>
       <c r="C102" s="7">
-        <v>-0.23</v>
+        <v>-0.24</v>
       </c>
       <c r="D102" s="3">
         <v>-0.04</v>
@@ -4868,21 +4991,21 @@
         <v>109</v>
       </c>
       <c r="H102" s="3">
-        <v>-0.09</v>
+        <v>-0.1</v>
       </c>
       <c r="I102" s="9">
         <v>113</v>
       </c>
       <c r="J102" s="18" t="s">
-        <v>157</v>
+        <v>154</v>
       </c>
     </row>
     <row r="103" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A103" s="5" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="B103">
-        <v>174</v>
+        <v>112</v>
       </c>
       <c r="C103" s="7">
         <v>-0.24</v>
@@ -4906,15 +5029,15 @@
         <v>56</v>
       </c>
       <c r="J103" s="18" t="s">
-        <v>158</v>
+        <v>155</v>
       </c>
     </row>
     <row r="104" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A104" s="5" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="B104">
-        <v>174</v>
+        <v>144</v>
       </c>
       <c r="C104" s="7">
         <v>-0.24</v>
@@ -4937,16 +5060,16 @@
       <c r="I104" s="9">
         <v>68</v>
       </c>
-      <c r="J104" s="17">
+      <c r="J104" s="18">
         <v>2</v>
       </c>
     </row>
     <row r="105" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A105" s="5" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="B105">
-        <v>174</v>
+        <v>192</v>
       </c>
       <c r="C105" s="7">
         <v>-0.25</v>
@@ -4970,7 +5093,7 @@
         <v>88</v>
       </c>
       <c r="J105" s="18" t="s">
-        <v>157</v>
+        <v>154</v>
       </c>
     </row>
     <row r="106" spans="1:10" x14ac:dyDescent="0.45">
@@ -4978,7 +5101,7 @@
         <v>34</v>
       </c>
       <c r="B106">
-        <v>174</v>
+        <v>160</v>
       </c>
       <c r="C106" s="7">
         <v>-0.25</v>
@@ -5007,10 +5130,10 @@
     </row>
     <row r="107" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A107" s="5" t="s">
-        <v>141</v>
+        <v>139</v>
       </c>
       <c r="B107">
-        <v>174</v>
+        <v>192</v>
       </c>
       <c r="C107" s="7">
         <v>-0.26</v>
@@ -5019,10 +5142,10 @@
         <v>-7.0000000000000007E-2</v>
       </c>
       <c r="E107" s="7">
-        <v>-0.19</v>
+        <v>-0.18</v>
       </c>
       <c r="F107" s="3">
-        <v>-0.02</v>
+        <v>-0.01</v>
       </c>
       <c r="G107" s="8">
         <v>92</v>
@@ -5033,16 +5156,16 @@
       <c r="I107" s="9">
         <v>100</v>
       </c>
-      <c r="J107" s="17">
+      <c r="J107" s="18">
         <v>2</v>
       </c>
     </row>
     <row r="108" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A108" s="5" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="B108">
-        <v>174</v>
+        <v>96</v>
       </c>
       <c r="C108" s="7">
         <v>-0.28000000000000003</v>
@@ -5066,15 +5189,15 @@
         <v>42</v>
       </c>
       <c r="J108" s="18" t="s">
-        <v>158</v>
+        <v>155</v>
       </c>
     </row>
     <row r="109" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A109" s="5" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="B109">
-        <v>174</v>
+        <v>192</v>
       </c>
       <c r="C109" s="7">
         <v>-0.28000000000000003</v>
@@ -5098,7 +5221,7 @@
         <v>105</v>
       </c>
       <c r="J109" s="18" t="s">
-        <v>158</v>
+        <v>155</v>
       </c>
     </row>
     <row r="110" spans="1:10" x14ac:dyDescent="0.45">
@@ -5106,19 +5229,19 @@
         <v>19</v>
       </c>
       <c r="B110">
-        <v>174</v>
+        <v>127</v>
       </c>
       <c r="C110" s="7">
         <v>-0.28000000000000003</v>
       </c>
       <c r="D110" s="3">
-        <v>-0.47</v>
+        <v>-0.48</v>
       </c>
       <c r="E110" s="7">
         <v>0.19</v>
       </c>
       <c r="F110" s="3">
-        <v>0.46</v>
+        <v>0.47</v>
       </c>
       <c r="G110" s="8">
         <v>65</v>
@@ -5135,16 +5258,16 @@
     </row>
     <row r="111" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A111" s="5" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="B111">
-        <v>174</v>
+        <v>192</v>
       </c>
       <c r="C111" s="7">
-        <v>-0.3</v>
+        <v>-0.28000000000000003</v>
       </c>
       <c r="D111" s="3">
-        <v>-0.24</v>
+        <v>-0.23</v>
       </c>
       <c r="E111" s="7">
         <v>-0.06</v>
@@ -5162,15 +5285,15 @@
         <v>101</v>
       </c>
       <c r="J111" s="18" t="s">
-        <v>157</v>
+        <v>154</v>
       </c>
     </row>
     <row r="112" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A112" s="5" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="B112">
-        <v>174</v>
+        <v>128</v>
       </c>
       <c r="C112" s="7">
         <v>-0.32</v>
@@ -5188,53 +5311,53 @@
         <v>61</v>
       </c>
       <c r="H112" s="3">
-        <v>0.01</v>
+        <v>0</v>
       </c>
       <c r="I112" s="9">
         <v>66</v>
       </c>
-      <c r="J112" s="16">
+      <c r="J112" s="18">
         <v>1</v>
       </c>
     </row>
     <row r="113" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A113" s="5" t="s">
-        <v>102</v>
+        <v>32</v>
       </c>
       <c r="B113">
-        <v>174</v>
+        <v>286</v>
       </c>
       <c r="C113" s="7">
-        <v>-0.33</v>
+        <v>-0.32</v>
       </c>
       <c r="D113" s="3">
-        <v>-0.75</v>
+        <v>-0.02</v>
       </c>
       <c r="E113" s="7">
-        <v>0.42</v>
+        <v>-0.3</v>
       </c>
       <c r="F113" s="3">
-        <v>1.01</v>
+        <v>-0.31</v>
       </c>
       <c r="G113" s="8">
-        <v>46</v>
+        <v>149</v>
       </c>
       <c r="H113" s="3">
-        <v>-0.14000000000000001</v>
+        <v>-0.3</v>
       </c>
       <c r="I113" s="9">
-        <v>48</v>
+        <v>135</v>
       </c>
       <c r="J113" s="18" t="s">
-        <v>158</v>
+        <v>23</v>
       </c>
     </row>
     <row r="114" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A114" s="5" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="B114">
-        <v>174</v>
+        <v>144</v>
       </c>
       <c r="C114" s="7">
         <v>-0.33</v>
@@ -5246,7 +5369,7 @@
         <v>-0.24</v>
       </c>
       <c r="F114" s="3">
-        <v>-0.06</v>
+        <v>-0.05</v>
       </c>
       <c r="G114" s="8">
         <v>77</v>
@@ -5257,28 +5380,28 @@
       <c r="I114" s="9">
         <v>67</v>
       </c>
-      <c r="J114" s="17">
+      <c r="J114" s="18">
         <v>2</v>
       </c>
     </row>
     <row r="115" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A115" s="5" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="B115">
-        <v>174</v>
+        <v>208</v>
       </c>
       <c r="C115" s="7">
         <v>-0.33</v>
       </c>
       <c r="D115" s="3">
-        <v>-0.15</v>
+        <v>-0.16</v>
       </c>
       <c r="E115" s="7">
         <v>-0.18</v>
       </c>
       <c r="F115" s="3">
-        <v>-0.19</v>
+        <v>-0.18</v>
       </c>
       <c r="G115" s="8">
         <v>124</v>
@@ -5289,40 +5412,40 @@
       <c r="I115" s="9">
         <v>83</v>
       </c>
-      <c r="J115" s="17">
+      <c r="J115" s="18">
         <v>2</v>
       </c>
     </row>
     <row r="116" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A116" s="5" t="s">
-        <v>32</v>
+        <v>101</v>
       </c>
       <c r="B116">
-        <v>174</v>
+        <v>95</v>
       </c>
       <c r="C116" s="7">
         <v>-0.33</v>
       </c>
       <c r="D116" s="3">
-        <v>-0.03</v>
+        <v>-0.75</v>
       </c>
       <c r="E116" s="7">
-        <v>-0.3</v>
+        <v>0.42</v>
       </c>
       <c r="F116" s="3">
-        <v>-0.31</v>
+        <v>1.01</v>
       </c>
       <c r="G116" s="8">
-        <v>149</v>
+        <v>46</v>
       </c>
       <c r="H116" s="3">
-        <v>-0.3</v>
+        <v>-0.14000000000000001</v>
       </c>
       <c r="I116" s="9">
-        <v>135</v>
+        <v>48</v>
       </c>
       <c r="J116" s="18" t="s">
-        <v>23</v>
+        <v>155</v>
       </c>
     </row>
     <row r="117" spans="1:10" x14ac:dyDescent="0.45">
@@ -5330,106 +5453,106 @@
         <v>105</v>
       </c>
       <c r="B117">
-        <v>174</v>
+        <v>176</v>
       </c>
       <c r="C117" s="7">
         <v>-0.34</v>
       </c>
       <c r="D117" s="3">
-        <v>-0.02</v>
+        <v>-0.04</v>
       </c>
       <c r="E117" s="7">
-        <v>-0.32</v>
+        <v>-0.3</v>
       </c>
       <c r="F117" s="3">
         <v>-0.14000000000000001</v>
       </c>
       <c r="G117" s="8">
-        <v>92</v>
+        <v>96</v>
       </c>
       <c r="H117" s="3">
-        <v>-0.53</v>
+        <v>-0.49</v>
       </c>
       <c r="I117" s="9">
-        <v>83</v>
-      </c>
-      <c r="J117" s="18" t="s">
-        <v>157</v>
+        <v>80</v>
+      </c>
+      <c r="J117" s="18">
+        <v>1</v>
       </c>
     </row>
     <row r="118" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A118" s="5" t="s">
-        <v>155</v>
+        <v>104</v>
       </c>
       <c r="B118">
-        <v>174</v>
+        <v>176</v>
       </c>
       <c r="C118" s="7">
         <v>-0.34</v>
       </c>
       <c r="D118" s="3">
-        <v>0.31</v>
+        <v>-0.02</v>
       </c>
       <c r="E118" s="7">
-        <v>-0.65</v>
+        <v>-0.32</v>
       </c>
       <c r="F118" s="3">
-        <v>-0.37</v>
+        <v>-0.14000000000000001</v>
       </c>
       <c r="G118" s="8">
-        <v>86</v>
+        <v>92</v>
       </c>
       <c r="H118" s="3">
-        <v>-0.88</v>
+        <v>-0.53</v>
       </c>
       <c r="I118" s="9">
-        <v>105</v>
+        <v>83</v>
       </c>
       <c r="J118" s="18" t="s">
-        <v>157</v>
+        <v>154</v>
       </c>
     </row>
     <row r="119" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A119" s="5" t="s">
-        <v>106</v>
+        <v>152</v>
       </c>
       <c r="B119">
-        <v>174</v>
+        <v>192</v>
       </c>
       <c r="C119" s="7">
         <v>-0.35</v>
       </c>
       <c r="D119" s="3">
-        <v>-0.05</v>
+        <v>0.3</v>
       </c>
       <c r="E119" s="7">
-        <v>-0.3</v>
+        <v>-0.65</v>
       </c>
       <c r="F119" s="3">
-        <v>-0.14000000000000001</v>
+        <v>-0.37</v>
       </c>
       <c r="G119" s="8">
-        <v>96</v>
+        <v>86</v>
       </c>
       <c r="H119" s="3">
-        <v>-0.49</v>
+        <v>-0.89</v>
       </c>
       <c r="I119" s="9">
-        <v>80</v>
-      </c>
-      <c r="J119" s="16">
-        <v>1</v>
+        <v>105</v>
+      </c>
+      <c r="J119" s="18" t="s">
+        <v>154</v>
       </c>
     </row>
     <row r="120" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A120" s="5" t="s">
-        <v>147</v>
+        <v>145</v>
       </c>
       <c r="B120">
-        <v>174</v>
+        <v>160</v>
       </c>
       <c r="C120" s="7">
-        <v>-0.39</v>
+        <v>-0.38</v>
       </c>
       <c r="D120" s="3">
         <v>-0.46</v>
@@ -5450,18 +5573,18 @@
         <v>74</v>
       </c>
       <c r="J120" s="18" t="s">
-        <v>157</v>
+        <v>154</v>
       </c>
     </row>
     <row r="121" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A121" s="5" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="B121">
-        <v>174</v>
+        <v>240</v>
       </c>
       <c r="C121" s="7">
-        <v>-0.42</v>
+        <v>-0.41</v>
       </c>
       <c r="D121" s="3">
         <v>-0.39</v>
@@ -5482,7 +5605,7 @@
         <v>112</v>
       </c>
       <c r="J121" s="18" t="s">
-        <v>158</v>
+        <v>155</v>
       </c>
     </row>
     <row r="122" spans="1:10" x14ac:dyDescent="0.45">
@@ -5490,7 +5613,7 @@
         <v>35</v>
       </c>
       <c r="B122">
-        <v>174</v>
+        <v>160</v>
       </c>
       <c r="C122" s="7">
         <v>-0.42</v>
@@ -5502,7 +5625,7 @@
         <v>-0.23</v>
       </c>
       <c r="F122" s="3">
-        <v>-0.49</v>
+        <v>-0.48</v>
       </c>
       <c r="G122" s="8">
         <v>70</v>
@@ -5522,62 +5645,62 @@
         <v>108</v>
       </c>
       <c r="B123">
-        <v>174</v>
+        <v>112</v>
       </c>
       <c r="C123" s="7">
-        <v>-0.46</v>
+        <v>-0.45</v>
       </c>
       <c r="D123" s="3">
-        <v>-0.33</v>
+        <v>0.1</v>
       </c>
       <c r="E123" s="7">
-        <v>-0.14000000000000001</v>
+        <v>-0.55000000000000004</v>
       </c>
       <c r="F123" s="3">
-        <v>-0.08</v>
+        <v>-0.64</v>
       </c>
       <c r="G123" s="8">
-        <v>97</v>
+        <v>61</v>
       </c>
       <c r="H123" s="3">
-        <v>-0.2</v>
+        <v>-0.44</v>
       </c>
       <c r="I123" s="9">
-        <v>94</v>
-      </c>
-      <c r="J123" s="17">
+        <v>51</v>
+      </c>
+      <c r="J123" s="18">
         <v>2</v>
       </c>
     </row>
     <row r="124" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A124" s="5" t="s">
-        <v>109</v>
+        <v>107</v>
       </c>
       <c r="B124">
-        <v>174</v>
+        <v>192</v>
       </c>
       <c r="C124" s="7">
         <v>-0.47</v>
       </c>
       <c r="D124" s="3">
-        <v>0.08</v>
+        <v>-0.33</v>
       </c>
       <c r="E124" s="7">
-        <v>-0.55000000000000004</v>
+        <v>-0.14000000000000001</v>
       </c>
       <c r="F124" s="3">
-        <v>-0.64</v>
+        <v>-0.08</v>
       </c>
       <c r="G124" s="8">
-        <v>61</v>
+        <v>97</v>
       </c>
       <c r="H124" s="3">
-        <v>-0.44</v>
+        <v>-0.2</v>
       </c>
       <c r="I124" s="9">
-        <v>51</v>
-      </c>
-      <c r="J124" s="17">
+        <v>94</v>
+      </c>
+      <c r="J124" s="18">
         <v>2</v>
       </c>
     </row>
@@ -5586,7 +5709,7 @@
         <v>20</v>
       </c>
       <c r="B125">
-        <v>174</v>
+        <v>176</v>
       </c>
       <c r="C125" s="7">
         <v>-0.47</v>
@@ -5598,13 +5721,13 @@
         <v>-0.45</v>
       </c>
       <c r="F125" s="3">
-        <v>-0.42</v>
+        <v>-0.41</v>
       </c>
       <c r="G125" s="8">
         <v>78</v>
       </c>
       <c r="H125" s="3">
-        <v>-0.49</v>
+        <v>-0.48</v>
       </c>
       <c r="I125" s="9">
         <v>97</v>
@@ -5615,22 +5738,22 @@
     </row>
     <row r="126" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A126" s="5" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="B126">
-        <v>174</v>
+        <v>238</v>
       </c>
       <c r="C126" s="7">
-        <v>-0.5</v>
+        <v>-0.49</v>
       </c>
       <c r="D126" s="3">
-        <v>-0.1</v>
+        <v>-0.09</v>
       </c>
       <c r="E126" s="7">
         <v>-0.4</v>
       </c>
       <c r="F126" s="3">
-        <v>-0.41</v>
+        <v>-0.4</v>
       </c>
       <c r="G126" s="8">
         <v>119</v>
@@ -5641,22 +5764,22 @@
       <c r="I126" s="9">
         <v>118</v>
       </c>
-      <c r="J126" s="17">
+      <c r="J126" s="18">
         <v>2</v>
       </c>
     </row>
     <row r="127" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A127" s="5" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="B127">
-        <v>174</v>
+        <v>192</v>
       </c>
       <c r="C127" s="7">
-        <v>-0.51</v>
+        <v>-0.52</v>
       </c>
       <c r="D127" s="3">
-        <v>-0.32</v>
+        <v>-0.33</v>
       </c>
       <c r="E127" s="7">
         <v>-0.18</v>
@@ -5668,33 +5791,33 @@
         <v>92</v>
       </c>
       <c r="H127" s="3">
-        <v>-0.35</v>
+        <v>-0.36</v>
       </c>
       <c r="I127" s="9">
         <v>99</v>
       </c>
-      <c r="J127" s="17">
+      <c r="J127" s="18">
         <v>2</v>
       </c>
     </row>
     <row r="128" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A128" s="5" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="B128">
-        <v>174</v>
+        <v>127</v>
       </c>
       <c r="C128" s="7">
         <v>-0.54</v>
       </c>
       <c r="D128" s="3">
-        <v>-0.6</v>
+        <v>-0.61</v>
       </c>
       <c r="E128" s="7">
-        <v>0.06</v>
+        <v>7.0000000000000007E-2</v>
       </c>
       <c r="F128" s="3">
-        <v>0.15</v>
+        <v>0.16</v>
       </c>
       <c r="G128" s="8">
         <v>67</v>
@@ -5705,7 +5828,7 @@
       <c r="I128" s="9">
         <v>60</v>
       </c>
-      <c r="J128" s="16">
+      <c r="J128" s="18">
         <v>1</v>
       </c>
     </row>
@@ -5714,7 +5837,7 @@
         <v>113</v>
       </c>
       <c r="B129">
-        <v>174</v>
+        <v>192</v>
       </c>
       <c r="C129" s="7">
         <v>-0.56999999999999995</v>
@@ -5726,27 +5849,27 @@
         <v>-0.17</v>
       </c>
       <c r="F129" s="3">
-        <v>-0.05</v>
+        <v>0.08</v>
       </c>
       <c r="G129" s="8">
-        <v>85</v>
+        <v>92</v>
       </c>
       <c r="H129" s="3">
-        <v>-0.28000000000000003</v>
+        <v>-0.39</v>
       </c>
       <c r="I129" s="9">
-        <v>91</v>
-      </c>
-      <c r="J129" s="18" t="s">
-        <v>157</v>
+        <v>99</v>
+      </c>
+      <c r="J129" s="18">
+        <v>2</v>
       </c>
     </row>
     <row r="130" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A130" s="5" t="s">
-        <v>114</v>
+        <v>112</v>
       </c>
       <c r="B130">
-        <v>174</v>
+        <v>176</v>
       </c>
       <c r="C130" s="7">
         <v>-0.56999999999999995</v>
@@ -5758,27 +5881,27 @@
         <v>-0.17</v>
       </c>
       <c r="F130" s="3">
-        <v>0.08</v>
+        <v>-0.05</v>
       </c>
       <c r="G130" s="8">
-        <v>92</v>
+        <v>85</v>
       </c>
       <c r="H130" s="3">
-        <v>-0.39</v>
+        <v>-0.28000000000000003</v>
       </c>
       <c r="I130" s="9">
-        <v>99</v>
-      </c>
-      <c r="J130" s="17">
-        <v>2</v>
+        <v>91</v>
+      </c>
+      <c r="J130" s="18" t="s">
+        <v>154</v>
       </c>
     </row>
     <row r="131" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A131" s="5" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="B131">
-        <v>174</v>
+        <v>192</v>
       </c>
       <c r="C131" s="7">
         <v>-0.62</v>
@@ -5802,15 +5925,15 @@
         <v>88</v>
       </c>
       <c r="J131" s="18" t="s">
-        <v>158</v>
+        <v>155</v>
       </c>
     </row>
     <row r="132" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A132" s="5" t="s">
-        <v>145</v>
+        <v>143</v>
       </c>
       <c r="B132">
-        <v>174</v>
+        <v>96</v>
       </c>
       <c r="C132" s="7">
         <v>-0.62</v>
@@ -5834,7 +5957,7 @@
         <v>50</v>
       </c>
       <c r="J132" s="18" t="s">
-        <v>158</v>
+        <v>155</v>
       </c>
     </row>
     <row r="133" spans="1:10" x14ac:dyDescent="0.45">
@@ -5842,10 +5965,10 @@
         <v>21</v>
       </c>
       <c r="B133">
-        <v>174</v>
+        <v>288</v>
       </c>
       <c r="C133" s="7">
-        <v>-0.65</v>
+        <v>-0.64</v>
       </c>
       <c r="D133" s="3">
         <v>-0.26</v>
@@ -5871,16 +5994,16 @@
     </row>
     <row r="134" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A134" s="5" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="B134">
-        <v>174</v>
+        <v>208</v>
       </c>
       <c r="C134" s="7">
         <v>-0.67</v>
       </c>
       <c r="D134" s="3">
-        <v>-0.42</v>
+        <v>-0.41</v>
       </c>
       <c r="E134" s="7">
         <v>-0.25</v>
@@ -5897,86 +6020,86 @@
       <c r="I134" s="9">
         <v>116</v>
       </c>
-      <c r="J134" s="17">
+      <c r="J134" s="18">
         <v>2</v>
       </c>
     </row>
     <row r="135" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A135" s="5" t="s">
-        <v>144</v>
+        <v>116</v>
       </c>
       <c r="B135">
-        <v>174</v>
+        <v>96</v>
       </c>
       <c r="C135" s="7">
         <v>-0.67</v>
       </c>
       <c r="D135" s="3">
-        <v>-0.51</v>
+        <v>0</v>
       </c>
       <c r="E135" s="7">
-        <v>-0.16</v>
+        <v>-0.66</v>
       </c>
       <c r="F135" s="3">
-        <v>-0.22</v>
+        <v>0.05</v>
       </c>
       <c r="G135" s="8">
-        <v>88</v>
+        <v>39</v>
       </c>
       <c r="H135" s="3">
-        <v>-0.11</v>
+        <v>-1.1499999999999999</v>
       </c>
       <c r="I135" s="9">
-        <v>103</v>
-      </c>
-      <c r="J135" s="16">
+        <v>57</v>
+      </c>
+      <c r="J135" s="18">
         <v>1</v>
       </c>
     </row>
     <row r="136" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A136" s="5" t="s">
-        <v>117</v>
+        <v>142</v>
       </c>
       <c r="B136">
-        <v>174</v>
+        <v>191</v>
       </c>
       <c r="C136" s="7">
-        <v>-0.67</v>
+        <v>-0.68</v>
       </c>
       <c r="D136" s="3">
-        <v>-0.01</v>
+        <v>-0.52</v>
       </c>
       <c r="E136" s="7">
-        <v>-0.66</v>
+        <v>-0.16</v>
       </c>
       <c r="F136" s="3">
-        <v>0.05</v>
+        <v>-0.22</v>
       </c>
       <c r="G136" s="8">
-        <v>39</v>
+        <v>88</v>
       </c>
       <c r="H136" s="3">
-        <v>-1.1499999999999999</v>
+        <v>-0.11</v>
       </c>
       <c r="I136" s="9">
-        <v>57</v>
-      </c>
-      <c r="J136" s="16">
+        <v>103</v>
+      </c>
+      <c r="J136" s="18">
         <v>1</v>
       </c>
     </row>
     <row r="137" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A137" s="5" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="B137">
-        <v>174</v>
+        <v>192</v>
       </c>
       <c r="C137" s="7">
-        <v>-0.69</v>
+        <v>-0.7</v>
       </c>
       <c r="D137" s="3">
-        <v>-0.41</v>
+        <v>-0.42</v>
       </c>
       <c r="E137" s="7">
         <v>-0.28000000000000003</v>
@@ -5994,15 +6117,15 @@
         <v>99</v>
       </c>
       <c r="J137" s="18" t="s">
-        <v>157</v>
+        <v>154</v>
       </c>
     </row>
     <row r="138" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A138" s="5" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="B138">
-        <v>174</v>
+        <v>176</v>
       </c>
       <c r="C138" s="7">
         <v>-0.71</v>
@@ -6014,27 +6137,27 @@
         <v>-0.18</v>
       </c>
       <c r="F138" s="3">
-        <v>-0.47</v>
+        <v>-0.46</v>
       </c>
       <c r="G138" s="8">
         <v>84</v>
       </c>
       <c r="H138" s="3">
-        <v>0.09</v>
+        <v>0.08</v>
       </c>
       <c r="I138" s="9">
         <v>92</v>
       </c>
-      <c r="J138" s="16">
+      <c r="J138" s="18">
         <v>1</v>
       </c>
     </row>
     <row r="139" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A139" s="5" t="s">
-        <v>146</v>
+        <v>144</v>
       </c>
       <c r="B139">
-        <v>174</v>
+        <v>192</v>
       </c>
       <c r="C139" s="7">
         <v>-0.72</v>
@@ -6058,7 +6181,7 @@
         <v>90</v>
       </c>
       <c r="J139" s="18" t="s">
-        <v>157</v>
+        <v>154</v>
       </c>
     </row>
     <row r="140" spans="1:10" x14ac:dyDescent="0.45">
@@ -6066,13 +6189,13 @@
         <v>22</v>
       </c>
       <c r="B140">
-        <v>174</v>
+        <v>191</v>
       </c>
       <c r="C140" s="7">
-        <v>-0.73</v>
+        <v>-0.75</v>
       </c>
       <c r="D140" s="3">
-        <v>-0.56999999999999995</v>
+        <v>-0.57999999999999996</v>
       </c>
       <c r="E140" s="7">
         <v>-0.17</v>
@@ -6084,7 +6207,7 @@
         <v>93</v>
       </c>
       <c r="H140" s="3">
-        <v>-0.3</v>
+        <v>-0.31</v>
       </c>
       <c r="I140" s="9">
         <v>97</v>
@@ -6095,22 +6218,22 @@
     </row>
     <row r="141" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A141" s="5" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="B141">
-        <v>174</v>
+        <v>160</v>
       </c>
       <c r="C141" s="7">
-        <v>-0.75</v>
+        <v>-0.76</v>
       </c>
       <c r="D141" s="3">
-        <v>-0.4</v>
+        <v>-0.41</v>
       </c>
       <c r="E141" s="7">
         <v>-0.35</v>
       </c>
       <c r="F141" s="3">
-        <v>-0.55000000000000004</v>
+        <v>-0.56000000000000005</v>
       </c>
       <c r="G141" s="8">
         <v>77</v>
@@ -6122,21 +6245,21 @@
         <v>82</v>
       </c>
       <c r="J141" s="18" t="s">
-        <v>158</v>
+        <v>155</v>
       </c>
     </row>
     <row r="142" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A142" s="5" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="B142">
-        <v>174</v>
+        <v>192</v>
       </c>
       <c r="C142" s="7">
         <v>-0.77</v>
       </c>
       <c r="D142" s="3">
-        <v>-0.52</v>
+        <v>-0.53</v>
       </c>
       <c r="E142" s="7">
         <v>-0.25</v>
@@ -6154,15 +6277,15 @@
         <v>100</v>
       </c>
       <c r="J142" s="18" t="s">
-        <v>157</v>
+        <v>154</v>
       </c>
     </row>
     <row r="143" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A143" s="5" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="B143">
-        <v>174</v>
+        <v>128</v>
       </c>
       <c r="C143" s="7">
         <v>-0.78</v>
@@ -6185,22 +6308,22 @@
       <c r="I143" s="9">
         <v>64</v>
       </c>
-      <c r="J143" s="16">
+      <c r="J143" s="18">
         <v>1</v>
       </c>
     </row>
     <row r="144" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A144" s="5" t="s">
-        <v>142</v>
+        <v>140</v>
       </c>
       <c r="B144">
-        <v>174</v>
+        <v>192</v>
       </c>
       <c r="C144" s="7">
-        <v>-0.8</v>
+        <v>-0.81</v>
       </c>
       <c r="D144" s="3">
-        <v>-0.33</v>
+        <v>-0.34</v>
       </c>
       <c r="E144" s="7">
         <v>-0.47</v>
@@ -6217,16 +6340,16 @@
       <c r="I144" s="9">
         <v>90</v>
       </c>
-      <c r="J144" s="16">
+      <c r="J144" s="18">
         <v>1</v>
       </c>
     </row>
     <row r="145" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A145" s="5" t="s">
-        <v>143</v>
+        <v>141</v>
       </c>
       <c r="B145">
-        <v>174</v>
+        <v>127</v>
       </c>
       <c r="C145" s="7">
         <v>-0.85</v>
@@ -6250,15 +6373,15 @@
         <v>60</v>
       </c>
       <c r="J145" s="18" t="s">
-        <v>158</v>
+        <v>155</v>
       </c>
     </row>
     <row r="146" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A146" s="5" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="B146">
-        <v>174</v>
+        <v>128</v>
       </c>
       <c r="C146" s="7">
         <v>-1.1499999999999999</v>
@@ -6267,10 +6390,10 @@
         <v>-0.74</v>
       </c>
       <c r="E146" s="7">
-        <v>-0.42</v>
+        <v>-0.41</v>
       </c>
       <c r="F146" s="3">
-        <v>-0.37</v>
+        <v>-0.35</v>
       </c>
       <c r="G146" s="8">
         <v>59</v>
@@ -6281,16 +6404,16 @@
       <c r="I146" s="9">
         <v>69</v>
       </c>
-      <c r="J146" s="16">
+      <c r="J146" s="18">
         <v>1</v>
       </c>
     </row>
     <row r="147" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A147" s="5" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="B147">
-        <v>174</v>
+        <v>171</v>
       </c>
       <c r="C147" s="7">
         <v>-1.22</v>
@@ -6313,7 +6436,7 @@
       <c r="I147" s="9">
         <v>91</v>
       </c>
-      <c r="J147" s="16">
+      <c r="J147" s="18">
         <v>1</v>
       </c>
     </row>
@@ -6321,6 +6444,40 @@
   <mergeCells count="1">
     <mergeCell ref="F1:I1"/>
   </mergeCells>
+  <conditionalFormatting sqref="J3">
+    <cfRule type="cellIs" dxfId="10" priority="6" operator="equal">
+      <formula>"3c"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="9" priority="7" operator="equal">
+      <formula>"3b"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="8" priority="8" operator="equal">
+      <formula>"3a"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="7" priority="9" operator="equal">
+      <formula>2</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="6" priority="10" operator="equal">
+      <formula>1</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="J4:J147">
+    <cfRule type="cellIs" dxfId="5" priority="1" operator="equal">
+      <formula>"3c"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="4" priority="2" operator="equal">
+      <formula>"3b"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="3" priority="3" operator="equal">
+      <formula>"3a"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="2" priority="4" operator="equal">
+      <formula>2</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="1" priority="5" operator="equal">
+      <formula>1</formula>
+    </cfRule>
+  </conditionalFormatting>
   <pageMargins left="0.23622047244094491" right="0.23622047244094491" top="0.74803149606299213" bottom="0.74803149606299213" header="0.31496062992125984" footer="0.31496062992125984"/>
   <pageSetup paperSize="9" scale="90" fitToHeight="0" orientation="portrait" r:id="rId1"/>
   <headerFooter>

</xml_diff>